<commit_message>
Modify AirSim Wrapper for PX4-MAVROS integration
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Missions" sheetId="1" state="visible" r:id="rId3"/>
@@ -761,7 +761,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -829,12 +829,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -930,7 +924,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -979,10 +973,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -995,7 +985,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1541,7 +1531,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="1" sqref="D5 D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1671,7 +1661,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" s="13" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>27</v>
       </c>
@@ -1681,7 +1671,7 @@
       <c r="C5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -1707,20 +1697,20 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="16"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1759,7 +1749,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="1" sqref="D5 D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1767,7 +1757,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="39.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="21" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="30.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="26.66"/>
@@ -1775,304 +1765,304 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="25" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="E3" s="27" t="n">
+      <c r="E3" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="27" t="n">
+      <c r="F3" s="26" t="n">
         <v>6.287</v>
       </c>
-      <c r="G3" s="27" t="n">
+      <c r="G3" s="26" t="n">
         <v>4.712</v>
       </c>
-      <c r="H3" s="27" t="n">
+      <c r="H3" s="26" t="n">
         <v>0.2</v>
       </c>
-      <c r="I3" s="27" t="n">
+      <c r="I3" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="J3" s="27" t="n">
+      <c r="J3" s="26" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="E4" s="27" t="n">
+      <c r="E4" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="F4" s="27" t="n">
+      <c r="F4" s="26" t="n">
         <v>13.2</v>
       </c>
-      <c r="G4" s="27" t="n">
+      <c r="G4" s="26" t="n">
         <v>8.8</v>
       </c>
-      <c r="H4" s="27" t="n">
+      <c r="H4" s="26" t="n">
         <v>0.5</v>
       </c>
-      <c r="I4" s="27" t="n">
+      <c r="I4" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="J4" s="27" t="n">
+      <c r="J4" s="26" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="E5" s="27" t="n">
+      <c r="E5" s="26" t="n">
         <v>30</v>
       </c>
-      <c r="F5" s="27" t="n">
+      <c r="F5" s="26" t="n">
         <v>35.9</v>
       </c>
-      <c r="G5" s="27" t="n">
+      <c r="G5" s="26" t="n">
         <v>24</v>
       </c>
-      <c r="H5" s="27" t="n">
+      <c r="H5" s="26" t="n">
         <v>0.6</v>
       </c>
-      <c r="I5" s="27" t="n">
+      <c r="I5" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="J5" s="27" t="n">
+      <c r="J5" s="26" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="E6" s="27" t="n">
+      <c r="E6" s="26" t="n">
         <v>15</v>
       </c>
-      <c r="F6" s="27" t="n">
+      <c r="F6" s="26" t="n">
         <v>17.3</v>
       </c>
-      <c r="G6" s="27" t="n">
+      <c r="G6" s="26" t="n">
         <v>13</v>
       </c>
-      <c r="H6" s="27" t="n">
+      <c r="H6" s="26" t="n">
         <v>0.5</v>
       </c>
-      <c r="I6" s="27" t="n">
+      <c r="I6" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="J6" s="27" t="n">
+      <c r="J6" s="26" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="E7" s="27" t="n">
+      <c r="E7" s="26" t="n">
         <v>14</v>
       </c>
-      <c r="F7" s="27" t="n">
+      <c r="F7" s="26" t="n">
         <v>6.287</v>
       </c>
-      <c r="G7" s="27" t="n">
+      <c r="G7" s="26" t="n">
         <v>4.712</v>
       </c>
-      <c r="H7" s="27" t="n">
+      <c r="H7" s="26" t="n">
         <v>0.4</v>
       </c>
-      <c r="I7" s="27" t="n">
+      <c r="I7" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="J7" s="27" t="n">
+      <c r="J7" s="26" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>232</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>233</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>234</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="E8" s="27" t="n">
+      <c r="E8" s="26" t="n">
         <v>10.27</v>
       </c>
-      <c r="F8" s="27" t="n">
+      <c r="F8" s="26" t="n">
         <v>13.2</v>
       </c>
-      <c r="G8" s="27" t="n">
+      <c r="G8" s="26" t="n">
         <v>8.8</v>
       </c>
-      <c r="H8" s="27" t="n">
+      <c r="H8" s="26" t="n">
         <v>0.5</v>
       </c>
-      <c r="I8" s="27" t="n">
+      <c r="I8" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="J8" s="27" t="n">
+      <c r="J8" s="26" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="E9" s="27" t="n">
+      <c r="E9" s="26" t="n">
         <v>5.5</v>
       </c>
-      <c r="F9" s="27" t="n">
+      <c r="F9" s="26" t="n">
         <v>6.3</v>
       </c>
-      <c r="G9" s="28" t="n">
+      <c r="G9" s="27" t="n">
         <v>4.7</v>
       </c>
-      <c r="H9" s="27" t="n">
+      <c r="H9" s="26" t="n">
         <v>0.8</v>
       </c>
-      <c r="I9" s="27" t="n">
+      <c r="I9" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="J9" s="27" t="n">
+      <c r="J9" s="26" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="10" s="13" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="s">
+    <row r="10" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="E10" s="27" t="n">
+      <c r="E10" s="26" t="n">
         <v>3.5</v>
       </c>
-      <c r="F10" s="27" t="n">
+      <c r="F10" s="26" t="n">
         <v>13.2</v>
       </c>
-      <c r="G10" s="27" t="n">
+      <c r="G10" s="26" t="n">
         <v>7.425</v>
       </c>
-      <c r="H10" s="27" t="n">
+      <c r="H10" s="26" t="n">
         <v>0.8</v>
       </c>
-      <c r="I10" s="27" t="n">
+      <c r="I10" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="J10" s="27" t="n">
+      <c r="J10" s="26" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2114,8 +2104,8 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2126,15 +2116,15 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
@@ -2170,9 +2160,9 @@
         <v>39</v>
       </c>
       <c r="D3" s="9" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E3" s="18" t="b">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="17" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2198,15 +2188,15 @@
       <c r="D4" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="18" t="b">
+      <c r="E4" s="17" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F4" s="18" t="b">
+      <c r="F4" s="17" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="18" t="b">
+      <c r="G4" s="17" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2222,39 +2212,39 @@
         <v>43</v>
       </c>
       <c r="D5" s="9" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E5" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="17" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F5" s="18" t="b">
+      <c r="F5" s="17" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G5" s="18" t="b">
+      <c r="G5" s="17" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C6" s="15"/>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C7" s="15"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16"/>
-      <c r="D9" s="15" t="s">
+      <c r="A9" s="15"/>
+      <c r="D9" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="15"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2291,7 +2281,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="1" sqref="D5 G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2303,15 +2293,15 @@
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -2355,7 +2345,7 @@
       <c r="F3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="18" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2384,7 +2374,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="1" sqref="D5 G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2394,15 +2384,15 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -2440,7 +2430,7 @@
       <c r="D3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="20" t="n">
+      <c r="E3" s="19" t="n">
         <v>16</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -2463,7 +2453,7 @@
       <c r="D4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="20" t="n">
+      <c r="E4" s="19" t="n">
         <v>16</v>
       </c>
       <c r="F4" s="9" t="s">
@@ -2505,13 +2495,13 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="1" sqref="D5 H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="21" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="20" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="29.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="32.44"/>
@@ -2520,263 +2510,263 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="M2" s="13"/>
+      <c r="M2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="24" t="n">
+      <c r="I3" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="J3" s="24" t="n">
+      <c r="J3" s="23" t="n">
         <v>250</v>
       </c>
-      <c r="K3" s="24" t="n">
+      <c r="K3" s="23" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="I4" s="24" t="n">
+      <c r="I4" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="J4" s="24" t="n">
+      <c r="J4" s="23" t="n">
         <v>250</v>
       </c>
-      <c r="K4" s="24" t="n">
+      <c r="K4" s="23" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="24" t="n">
+      <c r="I5" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="J5" s="24" t="n">
+      <c r="J5" s="23" t="n">
         <v>250</v>
       </c>
-      <c r="K5" s="24" t="n">
+      <c r="K5" s="23" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="I6" s="24" t="n">
+      <c r="I6" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="J6" s="24" t="n">
+      <c r="J6" s="23" t="n">
         <v>250</v>
       </c>
-      <c r="K6" s="24" t="n">
+      <c r="K6" s="23" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="I7" s="24" t="n">
+      <c r="I7" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="J7" s="24" t="n">
+      <c r="J7" s="23" t="n">
         <v>300</v>
       </c>
-      <c r="K7" s="24" t="n">
+      <c r="K7" s="23" t="n">
         <v>12000</v>
       </c>
     </row>
-    <row r="8" s="13" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="s">
+    <row r="8" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="I8" s="24" t="n">
+      <c r="I8" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="J8" s="24" t="n">
+      <c r="J8" s="23" t="n">
         <v>300</v>
       </c>
-      <c r="K8" s="24" t="n">
+      <c r="K8" s="23" t="n">
         <v>12000</v>
       </c>
       <c r="L8" s="2"/>
@@ -2823,13 +2813,13 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="topLeft" activeCell="I18" activeCellId="1" sqref="D5 I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="21" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="20" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="2" width="27.34"/>
@@ -2837,588 +2827,588 @@
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="22" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J3" s="24" t="n">
+      <c r="J3" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="K3" s="24" t="n">
+      <c r="K3" s="23" t="n">
         <v>0.5</v>
       </c>
-      <c r="L3" s="24" t="n">
+      <c r="L3" s="23" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="24" t="n">
+      <c r="J4" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="K4" s="24" t="n">
+      <c r="K4" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="L4" s="24" t="n">
+      <c r="L4" s="23" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="24" t="n">
+      <c r="J5" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="K5" s="24" t="n">
+      <c r="K5" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="L5" s="24" t="n">
+      <c r="L5" s="23" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="24" t="n">
+      <c r="J6" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="K6" s="24" t="n">
+      <c r="K6" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="L6" s="24" t="n">
+      <c r="L6" s="23" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="24" t="n">
+      <c r="J7" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="K7" s="24" t="n">
+      <c r="K7" s="23" t="n">
         <v>0.5</v>
       </c>
-      <c r="L7" s="24" t="n">
+      <c r="L7" s="23" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="24" t="n">
+      <c r="J8" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="K8" s="24" t="n">
+      <c r="K8" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="L8" s="24" t="n">
+      <c r="L8" s="23" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="24" t="n">
+      <c r="J9" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="K9" s="24" t="n">
+      <c r="K9" s="23" t="n">
         <v>0.5</v>
       </c>
-      <c r="L9" s="24" t="n">
+      <c r="L9" s="23" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J10" s="24" t="n">
+      <c r="J10" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="K10" s="24" t="n">
+      <c r="K10" s="23" t="n">
         <v>0.5</v>
       </c>
-      <c r="L10" s="24" t="n">
+      <c r="L10" s="23" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="I11" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J11" s="24" t="n">
+      <c r="J11" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="K11" s="24" t="n">
+      <c r="K11" s="23" t="n">
         <v>0.5</v>
       </c>
-      <c r="L11" s="24" t="n">
+      <c r="L11" s="23" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J12" s="24" t="n">
+      <c r="J12" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="K12" s="24" t="n">
+      <c r="K12" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="L12" s="24" t="n">
+      <c r="L12" s="23" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="I13" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J13" s="24" t="n">
+      <c r="J13" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="K13" s="24" t="n">
+      <c r="K13" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="L13" s="24" t="n">
+      <c r="L13" s="23" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="G14" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="24" t="n">
+      <c r="J14" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="K14" s="24" t="n">
+      <c r="K14" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="L14" s="24" t="n">
+      <c r="L14" s="23" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J15" s="24" t="n">
+      <c r="J15" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="K15" s="24" t="n">
+      <c r="K15" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="L15" s="24" t="n">
+      <c r="L15" s="23" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="16" s="13" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="s">
+    <row r="16" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="G16" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="J16" s="24" t="n">
+      <c r="J16" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="K16" s="24" t="n">
+      <c r="K16" s="23" t="n">
         <v>0.1</v>
       </c>
-      <c r="L16" s="24" t="n">
+      <c r="L16" s="23" t="n">
         <v>12</v>
       </c>
       <c r="M16" s="2"/>
@@ -3464,125 +3454,125 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="D5 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="21" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="20" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="2" width="26.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="2" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="25" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="27" t="n">
+      <c r="D3" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="27" t="n">
+      <c r="E3" s="26" t="n">
         <v>15</v>
       </c>
-      <c r="F3" s="27" t="n">
+      <c r="F3" s="26" t="n">
         <v>4.5</v>
       </c>
-      <c r="G3" s="27" t="n">
+      <c r="G3" s="26" t="n">
         <v>1.5</v>
       </c>
-      <c r="H3" s="27" t="n">
+      <c r="H3" s="26" t="n">
         <v>250</v>
       </c>
-      <c r="I3" s="27" t="n">
+      <c r="I3" s="26" t="n">
         <v>200</v>
       </c>
-      <c r="J3" s="27" t="n">
+      <c r="J3" s="26" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="D4" s="27" t="n">
+      <c r="D4" s="26" t="n">
         <v>8</v>
       </c>
-      <c r="E4" s="27" t="n">
+      <c r="E4" s="26" t="n">
         <v>12</v>
       </c>
-      <c r="F4" s="27" t="n">
+      <c r="F4" s="26" t="n">
         <v>6.5</v>
       </c>
-      <c r="G4" s="27" t="n">
+      <c r="G4" s="26" t="n">
         <v>2.5</v>
       </c>
-      <c r="H4" s="27" t="n">
+      <c r="H4" s="26" t="n">
         <v>400</v>
       </c>
-      <c r="I4" s="27" t="n">
+      <c r="I4" s="26" t="n">
         <v>350</v>
       </c>
-      <c r="J4" s="27" t="n">
+      <c r="J4" s="26" t="n">
         <v>25</v>
       </c>
     </row>
@@ -3627,7 +3617,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="1" sqref="D5 G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3637,82 +3627,82 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="E3" s="27" t="n">
+      <c r="E3" s="26" t="n">
         <v>0.4</v>
       </c>
-      <c r="F3" s="27" t="n">
+      <c r="F3" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="G3" s="27" t="n">
+      <c r="G3" s="26" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="E4" s="27" t="n">
+      <c r="E4" s="26" t="n">
         <v>0.6</v>
       </c>
-      <c r="F4" s="27" t="n">
+      <c r="F4" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="G4" s="27" t="n">
+      <c r="G4" s="26" t="n">
         <v>20</v>
       </c>
     </row>
@@ -3754,7 +3744,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="1" sqref="D5 J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3764,208 +3754,208 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="25" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="C3" s="27" t="n">
+      <c r="C3" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="F3" s="27" t="n">
+      <c r="F3" s="26" t="n">
         <v>50</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="H3" s="27" t="n">
+      <c r="H3" s="26" t="n">
         <v>270</v>
       </c>
-      <c r="I3" s="27" t="n">
+      <c r="I3" s="26" t="n">
         <v>0.06</v>
       </c>
-      <c r="J3" s="27" t="n">
+      <c r="J3" s="26" t="n">
         <v>0.95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="C4" s="27" t="n">
+      <c r="C4" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="F4" s="27" t="n">
+      <c r="F4" s="26" t="n">
         <v>50</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="H4" s="27" t="n">
+      <c r="H4" s="26" t="n">
         <v>180</v>
       </c>
-      <c r="I4" s="27" t="n">
+      <c r="I4" s="26" t="n">
         <v>0.05</v>
       </c>
-      <c r="J4" s="27" t="n">
+      <c r="J4" s="26" t="n">
         <v>0.97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="C5" s="27" t="n">
+      <c r="C5" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="F5" s="27" t="n">
+      <c r="F5" s="26" t="n">
         <v>50</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="H5" s="27" t="n">
+      <c r="H5" s="26" t="n">
         <v>270</v>
       </c>
-      <c r="I5" s="27" t="n">
+      <c r="I5" s="26" t="n">
         <v>0.06</v>
       </c>
-      <c r="J5" s="27" t="n">
+      <c r="J5" s="26" t="n">
         <v>0.95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="C6" s="27" t="n">
+      <c r="C6" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="F6" s="27" t="n">
+      <c r="F6" s="26" t="n">
         <v>50</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="H6" s="27" t="n">
+      <c r="H6" s="26" t="n">
         <v>180</v>
       </c>
-      <c r="I6" s="27" t="n">
+      <c r="I6" s="26" t="n">
         <v>0.1</v>
       </c>
-      <c r="J6" s="27" t="n">
+      <c r="J6" s="26" t="n">
         <v>0.97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="C7" s="27" t="n">
+      <c r="C7" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="F7" s="27" t="n">
+      <c r="F7" s="26" t="n">
         <v>50</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="H7" s="27" t="n">
+      <c r="H7" s="26" t="n">
         <v>180</v>
       </c>
-      <c r="I7" s="27" t="n">
+      <c r="I7" s="26" t="n">
         <v>0.05</v>
       </c>
-      <c r="J7" s="27" t="n">
+      <c r="J7" s="26" t="n">
         <v>0.99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solve issues regarding the target controller
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -1531,7 +1531,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="1" sqref="D5 D6"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1749,7 +1749,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="1" sqref="D5 D10"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2105,7 +2105,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2219,12 +2219,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="17" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="17" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2281,7 +2279,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="1" sqref="D5 G3"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2374,7 +2372,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="1" sqref="D5 G7"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2495,7 +2493,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="1" sqref="D5 H8"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2813,7 +2811,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="1" sqref="D5 I18"/>
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3455,7 +3453,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="D5 D9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3617,7 +3615,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="1" sqref="D5 G4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3744,7 +3742,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="1" sqref="D5 J7"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Solve out of view cropping when tracking targets
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Missions" sheetId="1" state="visible" r:id="rId3"/>
@@ -190,13 +190,13 @@
     <t xml:space="preserve">Coastal</t>
   </si>
   <si>
-    <t xml:space="preserve">(lat=47.64, lon=-122.14, alt=122.00)</t>
+    <t xml:space="preserve">(lat=35.9865559, lon=-5.8930106, alt=8.54)</t>
   </si>
   <si>
     <t xml:space="preserve">(13/12/2024)</t>
   </si>
   <si>
-    <t xml:space="preserve">(20:00:00)</t>
+    <t xml:space="preserve">(17:00:00)</t>
   </si>
   <si>
     <t xml:space="preserve">(Vx=0.0, Vy=0.0, Vz=0.0)</t>
@@ -749,7 +749,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -825,12 +825,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -918,7 +912,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1012,10 +1006,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1524,8 +1514,8 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1755,8 +1745,8 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1772,304 +1762,304 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="25" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="E3" s="27" t="n">
+      <c r="E3" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="27" t="n">
+      <c r="F3" s="26" t="n">
         <v>6.287</v>
       </c>
-      <c r="G3" s="27" t="n">
+      <c r="G3" s="26" t="n">
         <v>4.712</v>
       </c>
-      <c r="H3" s="27" t="n">
+      <c r="H3" s="26" t="n">
         <v>0.2</v>
       </c>
-      <c r="I3" s="27" t="n">
+      <c r="I3" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="J3" s="27" t="n">
+      <c r="J3" s="26" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="E4" s="27" t="n">
+      <c r="E4" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="F4" s="27" t="n">
+      <c r="F4" s="26" t="n">
         <v>13.2</v>
       </c>
-      <c r="G4" s="27" t="n">
+      <c r="G4" s="26" t="n">
         <v>8.8</v>
       </c>
-      <c r="H4" s="27" t="n">
+      <c r="H4" s="26" t="n">
         <v>0.5</v>
       </c>
-      <c r="I4" s="27" t="n">
+      <c r="I4" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="J4" s="27" t="n">
+      <c r="J4" s="26" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="E5" s="27" t="n">
+      <c r="E5" s="26" t="n">
         <v>30</v>
       </c>
-      <c r="F5" s="27" t="n">
+      <c r="F5" s="26" t="n">
         <v>35.9</v>
       </c>
-      <c r="G5" s="27" t="n">
+      <c r="G5" s="26" t="n">
         <v>24</v>
       </c>
-      <c r="H5" s="27" t="n">
+      <c r="H5" s="26" t="n">
         <v>0.6</v>
       </c>
-      <c r="I5" s="27" t="n">
+      <c r="I5" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="J5" s="27" t="n">
+      <c r="J5" s="26" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="E6" s="27" t="n">
+      <c r="E6" s="26" t="n">
         <v>15</v>
       </c>
-      <c r="F6" s="27" t="n">
+      <c r="F6" s="26" t="n">
         <v>17.3</v>
       </c>
-      <c r="G6" s="27" t="n">
+      <c r="G6" s="26" t="n">
         <v>13</v>
       </c>
-      <c r="H6" s="27" t="n">
+      <c r="H6" s="26" t="n">
         <v>0.5</v>
       </c>
-      <c r="I6" s="27" t="n">
+      <c r="I6" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="J6" s="27" t="n">
+      <c r="J6" s="26" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="E7" s="27" t="n">
+      <c r="E7" s="26" t="n">
         <v>14</v>
       </c>
-      <c r="F7" s="27" t="n">
+      <c r="F7" s="26" t="n">
         <v>6.287</v>
       </c>
-      <c r="G7" s="27" t="n">
+      <c r="G7" s="26" t="n">
         <v>4.712</v>
       </c>
-      <c r="H7" s="27" t="n">
+      <c r="H7" s="26" t="n">
         <v>0.4</v>
       </c>
-      <c r="I7" s="27" t="n">
+      <c r="I7" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="J7" s="27" t="n">
+      <c r="J7" s="26" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="E8" s="27" t="n">
+      <c r="E8" s="26" t="n">
         <v>10.27</v>
       </c>
-      <c r="F8" s="27" t="n">
+      <c r="F8" s="26" t="n">
         <v>13.2</v>
       </c>
-      <c r="G8" s="27" t="n">
+      <c r="G8" s="26" t="n">
         <v>8.8</v>
       </c>
-      <c r="H8" s="27" t="n">
+      <c r="H8" s="26" t="n">
         <v>0.5</v>
       </c>
-      <c r="I8" s="27" t="n">
+      <c r="I8" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="J8" s="27" t="n">
+      <c r="J8" s="26" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>232</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="26" t="s">
         <v>233</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="E9" s="27" t="n">
+      <c r="E9" s="26" t="n">
         <v>5.5</v>
       </c>
-      <c r="F9" s="27" t="n">
+      <c r="F9" s="26" t="n">
         <v>6.3</v>
       </c>
-      <c r="G9" s="28" t="n">
+      <c r="G9" s="27" t="n">
         <v>4.7</v>
       </c>
-      <c r="H9" s="27" t="n">
+      <c r="H9" s="26" t="n">
         <v>0.8</v>
       </c>
-      <c r="I9" s="27" t="n">
+      <c r="I9" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="J9" s="27" t="n">
+      <c r="J9" s="26" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="10" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>234</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="E10" s="27" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="F10" s="27" t="n">
+      <c r="E10" s="26" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F10" s="26" t="n">
         <v>13.2</v>
       </c>
-      <c r="G10" s="27" t="n">
+      <c r="G10" s="26" t="n">
         <v>7.425</v>
       </c>
-      <c r="H10" s="27" t="n">
+      <c r="H10" s="26" t="n">
         <v>0.8</v>
       </c>
-      <c r="I10" s="27" t="n">
+      <c r="I10" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="J10" s="27" t="n">
+      <c r="J10" s="26" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2287,8 +2277,8 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3363,7 +3353,7 @@
       <c r="C16" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="23" t="s">
         <v>131</v>
       </c>
       <c r="E16" s="23" t="s">
@@ -3444,112 +3434,112 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="25" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="27" t="n">
+      <c r="D3" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="27" t="n">
+      <c r="E3" s="26" t="n">
         <v>15</v>
       </c>
-      <c r="F3" s="27" t="n">
+      <c r="F3" s="26" t="n">
         <v>4.5</v>
       </c>
-      <c r="G3" s="27" t="n">
+      <c r="G3" s="26" t="n">
         <v>1.5</v>
       </c>
-      <c r="H3" s="27" t="n">
+      <c r="H3" s="26" t="n">
         <v>250</v>
       </c>
-      <c r="I3" s="27" t="n">
+      <c r="I3" s="26" t="n">
         <v>200</v>
       </c>
-      <c r="J3" s="27" t="n">
+      <c r="J3" s="26" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="D4" s="27" t="n">
+      <c r="D4" s="26" t="n">
         <v>8</v>
       </c>
-      <c r="E4" s="27" t="n">
+      <c r="E4" s="26" t="n">
         <v>12</v>
       </c>
-      <c r="F4" s="27" t="n">
+      <c r="F4" s="26" t="n">
         <v>6.5</v>
       </c>
-      <c r="G4" s="27" t="n">
+      <c r="G4" s="26" t="n">
         <v>2.5</v>
       </c>
-      <c r="H4" s="27" t="n">
+      <c r="H4" s="26" t="n">
         <v>400</v>
       </c>
-      <c r="I4" s="27" t="n">
+      <c r="I4" s="26" t="n">
         <v>350</v>
       </c>
-      <c r="J4" s="27" t="n">
+      <c r="J4" s="26" t="n">
         <v>25</v>
       </c>
     </row>
@@ -3606,73 +3596,73 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>188</v>
       </c>
       <c r="G2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="D3" s="27" t="n">
+      <c r="D3" s="26" t="n">
         <v>0.4</v>
       </c>
-      <c r="E3" s="27" t="n">
+      <c r="E3" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="F3" s="27" t="n">
+      <c r="F3" s="26" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="D4" s="27" t="n">
+      <c r="D4" s="26" t="n">
         <v>0.6</v>
       </c>
-      <c r="E4" s="27" t="n">
+      <c r="E4" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="F4" s="27" t="n">
+      <c r="F4" s="26" t="n">
         <v>20</v>
       </c>
     </row>
@@ -3727,36 +3717,36 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>198</v>
       </c>
       <c r="H2" s="20"/>
@@ -3764,117 +3754,117 @@
       <c r="J2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="E3" s="27" t="n">
+      <c r="E3" s="26" t="n">
         <v>180</v>
       </c>
-      <c r="F3" s="27" t="n">
+      <c r="F3" s="26" t="n">
         <v>0.1</v>
       </c>
-      <c r="G3" s="27" t="n">
+      <c r="G3" s="26" t="n">
         <v>0.97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="E4" s="27" t="n">
+      <c r="E4" s="26" t="n">
         <v>180</v>
       </c>
-      <c r="F4" s="27" t="n">
+      <c r="F4" s="26" t="n">
         <v>0.05</v>
       </c>
-      <c r="G4" s="27" t="n">
+      <c r="G4" s="26" t="n">
         <v>0.99</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="E5" s="27" t="n">
+      <c r="E5" s="26" t="n">
         <v>270</v>
       </c>
-      <c r="F5" s="27" t="n">
+      <c r="F5" s="26" t="n">
         <v>0.06</v>
       </c>
-      <c r="G5" s="27" t="n">
+      <c r="G5" s="26" t="n">
         <v>0.95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="E6" s="27" t="n">
+      <c r="E6" s="26" t="n">
         <v>180</v>
       </c>
-      <c r="F6" s="27" t="n">
+      <c r="F6" s="26" t="n">
         <v>0.1</v>
       </c>
-      <c r="G6" s="27" t="n">
+      <c r="G6" s="26" t="n">
         <v>0.97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="E7" s="27" t="n">
+      <c r="E7" s="26" t="n">
         <v>180</v>
       </c>
-      <c r="F7" s="27" t="n">
+      <c r="F7" s="26" t="n">
         <v>0.05</v>
       </c>
-      <c r="G7" s="27" t="n">
+      <c r="G7" s="26" t="n">
         <v>0.99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add noise settings for cameras
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="240">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -679,6 +679,12 @@
     <t xml:space="preserve">SensorHeight [mm]</t>
   </si>
   <si>
+    <t xml:space="preserve">LensDistortion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RandomNoise</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raspberry Pi Camera HQ Lens 2.8 12mm</t>
   </si>
   <si>
@@ -686,6 +692,12 @@
   </si>
   <si>
     <t xml:space="preserve">(2560x1440)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Strength=0.025, Radius=2.0, Falloff=0.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(RandContrib=0.01, RandSize=500, RandSpeed=50000)</t>
   </si>
   <si>
     <t xml:space="preserve">Mavic 2 Pro (Mod. Zoom)</t>
@@ -1227,9 +1239,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table29" displayName="Table29" ref="A2:J9" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:J9"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table29" displayName="Table29" ref="A2:L9" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:L9"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="CameraModelID"/>
     <tableColumn id="2" name="CameraName"/>
     <tableColumn id="3" name="CameraType"/>
@@ -1237,9 +1249,11 @@
     <tableColumn id="5" name="DefaultFocal [mm]"/>
     <tableColumn id="6" name="SensorWidth [mm]"/>
     <tableColumn id="7" name="SensorHeight [mm]"/>
-    <tableColumn id="8" name="Weight [kg]"/>
-    <tableColumn id="9" name="IdlePower [W]"/>
-    <tableColumn id="10" name="ActivePower [W]"/>
+    <tableColumn id="8" name="LensDistortion"/>
+    <tableColumn id="9" name="RandomNoise"/>
+    <tableColumn id="10" name="Weight [kg]"/>
+    <tableColumn id="11" name="IdlePower [W]"/>
+    <tableColumn id="12" name="ActivePower [W]"/>
   </tableColumns>
 </table>
 </file>
@@ -1743,10 +1757,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1755,10 +1769,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="39.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="30.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="2" width="51.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="30.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="13" style="2" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1774,6 +1790,8 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
@@ -1798,12 +1816,18 @@
         <v>215</v>
       </c>
       <c r="H2" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="K2" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="L2" s="25" t="s">
         <v>188</v>
       </c>
     </row>
@@ -1812,13 +1836,13 @@
         <v>125</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E3" s="26" t="n">
         <v>1</v>
@@ -1829,13 +1853,19 @@
       <c r="G3" s="26" t="n">
         <v>4.712</v>
       </c>
-      <c r="H3" s="26" t="n">
+      <c r="H3" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="26" t="n">
         <v>0.2</v>
       </c>
-      <c r="I3" s="26" t="n">
+      <c r="K3" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="J3" s="26" t="n">
+      <c r="L3" s="26" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1844,13 +1874,13 @@
         <v>132</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>217</v>
-      </c>
       <c r="D4" s="26" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E4" s="26" t="n">
         <v>10</v>
@@ -1861,28 +1891,34 @@
       <c r="G4" s="26" t="n">
         <v>8.8</v>
       </c>
-      <c r="H4" s="26" t="n">
+      <c r="H4" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="J4" s="26" t="n">
         <v>0.5</v>
       </c>
-      <c r="I4" s="26" t="n">
+      <c r="K4" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="J4" s="26" t="n">
+      <c r="L4" s="26" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E5" s="26" t="n">
         <v>30</v>
@@ -1893,28 +1929,34 @@
       <c r="G5" s="26" t="n">
         <v>24</v>
       </c>
-      <c r="H5" s="26" t="n">
+      <c r="H5" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="J5" s="26" t="n">
         <v>0.6</v>
       </c>
-      <c r="I5" s="26" t="n">
+      <c r="K5" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="J5" s="26" t="n">
+      <c r="L5" s="26" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B6" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>224</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>220</v>
       </c>
       <c r="E6" s="26" t="n">
         <v>15</v>
@@ -1925,28 +1967,34 @@
       <c r="G6" s="26" t="n">
         <v>13</v>
       </c>
-      <c r="H6" s="26" t="n">
+      <c r="H6" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="J6" s="26" t="n">
         <v>0.5</v>
       </c>
-      <c r="I6" s="26" t="n">
+      <c r="K6" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="J6" s="26" t="n">
+      <c r="L6" s="26" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E7" s="26" t="n">
         <v>14</v>
@@ -1957,28 +2005,34 @@
       <c r="G7" s="26" t="n">
         <v>4.712</v>
       </c>
-      <c r="H7" s="26" t="n">
+      <c r="H7" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="J7" s="26" t="n">
         <v>0.4</v>
       </c>
-      <c r="I7" s="26" t="n">
+      <c r="K7" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="J7" s="26" t="n">
+      <c r="L7" s="26" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="E8" s="26" t="n">
         <v>10.27</v>
@@ -1989,28 +2043,34 @@
       <c r="G8" s="26" t="n">
         <v>8.8</v>
       </c>
-      <c r="H8" s="26" t="n">
+      <c r="H8" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="J8" s="26" t="n">
         <v>0.5</v>
       </c>
-      <c r="I8" s="26" t="n">
+      <c r="K8" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="J8" s="26" t="n">
+      <c r="L8" s="26" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="26" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="E9" s="26" t="n">
         <v>5.5</v>
@@ -2021,13 +2081,19 @@
       <c r="G9" s="27" t="n">
         <v>4.7</v>
       </c>
-      <c r="H9" s="26" t="n">
+      <c r="H9" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="J9" s="26" t="n">
         <v>0.8</v>
       </c>
-      <c r="I9" s="26" t="n">
+      <c r="K9" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="J9" s="26" t="n">
+      <c r="L9" s="26" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2036,13 +2102,13 @@
         <v>168</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E10" s="26" t="n">
         <v>4.5</v>
@@ -2053,13 +2119,19 @@
       <c r="G10" s="26" t="n">
         <v>7.425</v>
       </c>
-      <c r="H10" s="26" t="n">
+      <c r="H10" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="J10" s="26" t="n">
         <v>0.8</v>
       </c>
-      <c r="I10" s="26" t="n">
+      <c r="K10" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="J10" s="26" t="n">
+      <c r="L10" s="26" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2079,7 +2151,7 @@
     <row r="24" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Add support for multiple vehicle types
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -133,6 +133,9 @@
     <t xml:space="preserve">TEAM02</t>
   </si>
   <si>
+    <t xml:space="preserve">PX4</t>
+  </si>
+  <si>
     <t xml:space="preserve">SimulationName</t>
   </si>
   <si>
@@ -163,9 +166,6 @@
     <t xml:space="preserve">Regular PX4</t>
   </si>
   <si>
-    <t xml:space="preserve">PX4</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -391,7 +391,10 @@
     <t xml:space="preserve">PAYLOAD05</t>
   </si>
   <si>
-    <t xml:space="preserve">(X=15.0, Y=20.0, Z=100.0)</t>
+    <t xml:space="preserve">DRONE01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=0.0, Z=0.0)</t>
   </si>
   <si>
     <t xml:space="preserve">HeadID</t>
@@ -602,9 +605,6 @@
   </si>
   <si>
     <t xml:space="preserve">Quadcopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DRONE01</t>
   </si>
   <si>
     <t xml:space="preserve">Default Hexacopter</t>
@@ -1563,7 +1563,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1729,7 +1729,7 @@
         <v>33</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>28</v>
@@ -1813,7 +1813,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>220</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>228</v>
@@ -1905,7 +1905,7 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>233</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="10" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="26" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>248</v>
@@ -2235,25 +2235,25 @@
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2261,7 +2261,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>20</v>
@@ -2288,10 +2288,10 @@
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>20</v>
@@ -2321,10 +2321,10 @@
         <v>32</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>1</v>
@@ -2613,8 +2613,8 @@
   </sheetPr>
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N14" activeCellId="0" sqref="N14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2952,10 +2952,10 @@
         <v>91</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H8" s="23" t="s">
         <v>94</v>
@@ -3056,64 +3056,64 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>90</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I3" s="23" t="n">
         <v>2</v>
@@ -3128,28 +3128,28 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>90</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I4" s="23" t="n">
         <v>10</v>
@@ -3164,28 +3164,28 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>90</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I5" s="23" t="n">
         <v>10</v>
@@ -3200,28 +3200,28 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>90</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I6" s="23" t="n">
         <v>10</v>
@@ -3236,28 +3236,28 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>101</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I7" s="23" t="n">
         <v>2</v>
@@ -3272,28 +3272,28 @@
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>101</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I8" s="23" t="n">
         <v>10</v>
@@ -3308,28 +3308,28 @@
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>105</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I9" s="23" t="n">
         <v>2</v>
@@ -3344,28 +3344,28 @@
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I10" s="23" t="n">
         <v>2</v>
@@ -3380,28 +3380,28 @@
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>115</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I11" s="23" t="n">
         <v>2</v>
@@ -3416,28 +3416,28 @@
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>115</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I12" s="23" t="n">
         <v>10</v>
@@ -3452,28 +3452,28 @@
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>115</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I13" s="23" t="n">
         <v>10</v>
@@ -3488,28 +3488,28 @@
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>115</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H14" s="23" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I14" s="23" t="n">
         <v>10</v>
@@ -3524,28 +3524,28 @@
     </row>
     <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>115</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H15" s="23" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I15" s="23" t="n">
         <v>10</v>
@@ -3560,28 +3560,28 @@
     </row>
     <row r="16" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>119</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I16" s="23" t="n">
         <v>2</v>
@@ -3637,7 +3637,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3650,7 +3650,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3667,31 +3667,31 @@
         <v>78</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3699,10 +3699,10 @@
         <v>92</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D3" s="26" t="n">
         <v>10</v>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>191</v>
+        <v>120</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>192</v>
@@ -3812,7 +3812,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>194</v>
@@ -3843,7 +3843,7 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>199</v>
@@ -3863,7 +3863,7 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>201</v>
@@ -3933,7 +3933,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>

</xml_diff>

<commit_message>
Quick fixes (GUI, target and cluster spawn, camera sensor noise...)
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Missions" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="266">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -154,6 +154,12 @@
     <t xml:space="preserve">ClockSpeed</t>
   </si>
   <si>
+    <t xml:space="preserve">ScenarioViewPosition [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ScenarioViewOrientation [°]</t>
+  </si>
+  <si>
     <t xml:space="preserve">RecordMetrics</t>
   </si>
   <si>
@@ -169,6 +175,12 @@
     <t xml:space="preserve">Slow Simple</t>
   </si>
   <si>
+    <t xml:space="preserve">(X=-150.0, Y=-150.0, Z=150.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=15.0, Yaw=45.0, Roll=0.0)</t>
+  </si>
+  <si>
     <t xml:space="preserve">SIM01</t>
   </si>
   <si>
@@ -178,6 +190,9 @@
     <t xml:space="preserve">Regular PX4</t>
   </si>
   <si>
+    <t xml:space="preserve">(X=-250.0, Y=-250.0, Z=150.0)</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -220,9 +235,6 @@
     <t xml:space="preserve">Coastal</t>
   </si>
   <si>
-    <t xml:space="preserve">(19:00:00)</t>
-  </si>
-  <si>
     <t xml:space="preserve">GroupID</t>
   </si>
   <si>
@@ -274,6 +286,9 @@
     <t xml:space="preserve">MetaHuman</t>
   </si>
   <si>
+    <t xml:space="preserve">VeyLowSpeedHighDispersion16</t>
+  </si>
+  <si>
     <t xml:space="preserve">AGENT CONFIGURATION</t>
   </si>
   <si>
@@ -583,18 +598,39 @@
     <t xml:space="preserve">MaxSpeed [m/s]</t>
   </si>
   <si>
+    <t xml:space="preserve">EnableBarometer</t>
+  </si>
+  <si>
     <t xml:space="preserve">Barometer</t>
   </si>
   <si>
+    <t xml:space="preserve">EnableIMU</t>
+  </si>
+  <si>
     <t xml:space="preserve">IMU</t>
   </si>
   <si>
+    <t xml:space="preserve">EnableGPS</t>
+  </si>
+  <si>
     <t xml:space="preserve">GPS</t>
   </si>
   <si>
+    <t xml:space="preserve">EnableMagnetometer</t>
+  </si>
+  <si>
     <t xml:space="preserve">Magnetometer</t>
   </si>
   <si>
+    <t xml:space="preserve">BaseWeight [kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxPayloadWeight [kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HoverPower [W]</t>
+  </si>
+  <si>
     <t xml:space="preserve">CruisePower [W]</t>
   </si>
   <si>
@@ -607,16 +643,16 @@
     <t xml:space="preserve">Quadcopter</t>
   </si>
   <si>
-    <t xml:space="preserve">(Enabled=false, PressureSigma=0.0001825, NoiseSigma=3.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Enabled=true, GyroNoise=0.4, AccelNoise=0.2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Enabled=true, EphIni=30, EpvIni=40, EphFin=1, EpvFin=2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Enabled=false, NoiseSigma=0.03, ScaleFactor=1.02, NoiseBias=0.05)</t>
+    <t xml:space="preserve">(PressureSigma=0.0001825, NoiseSigma=3.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(GyroNoise=0.4, AccelNoise=0.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(EphIni=30, EpvIni=40, EphFin=1, EpvFin=2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(NoiseSigma=0.03, ScaleFactor=1.02, NoiseBias=0.05)</t>
   </si>
   <si>
     <t xml:space="preserve">DJI S900</t>
@@ -721,10 +757,16 @@
     <t xml:space="preserve">SensorHeight [mm]</t>
   </si>
   <si>
+    <t xml:space="preserve">EnableLensDistortion</t>
+  </si>
+  <si>
     <t xml:space="preserve">LensDistortion</t>
   </si>
   <si>
-    <t xml:space="preserve">RandomNoise</t>
+    <t xml:space="preserve">EnableSensorNoise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SensorNoise</t>
   </si>
   <si>
     <t xml:space="preserve">Raspberry Pi Camera HQ Lens 2.8 12mm</t>
@@ -736,10 +778,10 @@
     <t xml:space="preserve">(2560x1440)</t>
   </si>
   <si>
-    <t xml:space="preserve">(Enabled=true, Strength=0.025, Radius=2.0, Falloff=0.2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Enabled=true, RandContrib=0.01, RandSize=500, RandSpeed=50000)</t>
+    <t xml:space="preserve">(Strength=0.02, Radius=1.8, Falloff=0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(RandContrib=0.008, RandSize=500, RandSpeed=50000)</t>
   </si>
   <si>
     <t xml:space="preserve">Mavic 2 Pro (Mod. Zoom)</t>
@@ -797,7 +839,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -873,12 +915,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -966,7 +1002,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1051,10 +1087,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1080,10 +1112,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1288,9 +1316,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table29" displayName="Table29" ref="A2:L9" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:L9"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table29" displayName="Table29" ref="A2:N9" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:N9"/>
+  <tableColumns count="14">
     <tableColumn id="1" name="CameraModelID"/>
     <tableColumn id="2" name="CameraName"/>
     <tableColumn id="3" name="CameraType"/>
@@ -1298,11 +1326,13 @@
     <tableColumn id="5" name="DefaultFocal [mm]"/>
     <tableColumn id="6" name="SensorWidth [mm]"/>
     <tableColumn id="7" name="SensorHeight [mm]"/>
-    <tableColumn id="8" name="LensDistortion"/>
-    <tableColumn id="9" name="RandomNoise"/>
-    <tableColumn id="10" name="Weight [kg]"/>
-    <tableColumn id="11" name="IdlePower [W]"/>
-    <tableColumn id="12" name="ActivePower [W]"/>
+    <tableColumn id="8" name="EnableLensDistortion"/>
+    <tableColumn id="9" name="LensDistortion"/>
+    <tableColumn id="10" name="EnableSensorNoise"/>
+    <tableColumn id="11" name="SensorNoise"/>
+    <tableColumn id="12" name="Weight [kg]"/>
+    <tableColumn id="13" name="IdlePower [W]"/>
+    <tableColumn id="14" name="ActivePower [W]"/>
   </tableColumns>
 </table>
 </file>
@@ -1337,20 +1367,27 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table2913" displayName="Table2913" ref="A2:K4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:K4"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table2913" displayName="Table2913" ref="A2:R4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:R4"/>
+  <tableColumns count="18">
     <tableColumn id="1" name="DroneModelID"/>
     <tableColumn id="2" name="DroneName"/>
     <tableColumn id="3" name="DroneType"/>
     <tableColumn id="4" name="CruiseSpeed [m/s]"/>
     <tableColumn id="5" name="MaxSpeed [m/s]"/>
-    <tableColumn id="6" name="Barometer"/>
-    <tableColumn id="7" name="IMU"/>
-    <tableColumn id="8" name="GPS"/>
-    <tableColumn id="9" name="Magnetometer"/>
-    <tableColumn id="10" name="CruisePower [W]"/>
-    <tableColumn id="11" name="LoadFactor [W/kg]"/>
+    <tableColumn id="6" name="EnableBarometer"/>
+    <tableColumn id="7" name="Barometer"/>
+    <tableColumn id="8" name="EnableIMU"/>
+    <tableColumn id="9" name="IMU"/>
+    <tableColumn id="10" name="EnableGPS"/>
+    <tableColumn id="11" name="GPS"/>
+    <tableColumn id="12" name="EnableMagnetometer"/>
+    <tableColumn id="13" name="Magnetometer"/>
+    <tableColumn id="14" name="BaseWeight [kg]"/>
+    <tableColumn id="15" name="MaxPayloadWeight [kg]"/>
+    <tableColumn id="16" name="HoverPower [W]"/>
+    <tableColumn id="17" name="CruisePower [W]"/>
+    <tableColumn id="18" name="LoadFactor [W/kg]"/>
   </tableColumns>
 </table>
 </file>
@@ -1386,14 +1423,16 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table7" displayName="Table7" ref="A2:E5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:E5"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table7" displayName="Table7" ref="A2:G5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:G5"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="SimulationID"/>
     <tableColumn id="2" name="SimulationName"/>
     <tableColumn id="3" name="ClockSpeed"/>
-    <tableColumn id="4" name="RecordMetrics"/>
-    <tableColumn id="5" name="DrawRvizMarkers"/>
+    <tableColumn id="4" name="ScenarioViewPosition [m]"/>
+    <tableColumn id="5" name="ScenarioViewOrientation [°]"/>
+    <tableColumn id="6" name="RecordMetrics"/>
+    <tableColumn id="7" name="DrawRvizMarkers"/>
   </tableColumns>
 </table>
 </file>
@@ -1577,8 +1616,8 @@
   </sheetPr>
   <dimension ref="A1:XFD20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1823,10 +1862,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1836,368 +1875,443 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="2" width="68.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="30.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="32.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="68.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="30.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="68.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="13" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="30.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="15" style="2" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
+      <c r="A1" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>227</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="J2" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="K2" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="L2" s="26" t="s">
-        <v>202</v>
+      <c r="A2" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="E3" s="27" t="n">
+      <c r="A3" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="27" t="n">
+      <c r="F3" s="26" t="n">
         <v>6.287</v>
       </c>
-      <c r="G3" s="27" t="n">
+      <c r="G3" s="26" t="n">
         <v>4.712</v>
       </c>
-      <c r="H3" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="J3" s="27" t="n">
+      <c r="H3" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="J3" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="L3" s="26" t="n">
         <v>0.2</v>
       </c>
-      <c r="K3" s="27" t="n">
+      <c r="M3" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="L3" s="27" t="n">
+      <c r="N3" s="26" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="E4" s="27" t="n">
+      <c r="A4" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="E4" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="F4" s="27" t="n">
+      <c r="F4" s="26" t="n">
         <v>13.2</v>
       </c>
-      <c r="G4" s="27" t="n">
+      <c r="G4" s="26" t="n">
         <v>8.8</v>
       </c>
-      <c r="H4" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="J4" s="27" t="n">
+      <c r="H4" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="J4" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="L4" s="26" t="n">
         <v>0.5</v>
       </c>
-      <c r="K4" s="27" t="n">
+      <c r="M4" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="L4" s="27" t="n">
+      <c r="N4" s="26" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
-        <v>239</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>240</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="E5" s="27" t="n">
+      <c r="A5" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="E5" s="26" t="n">
         <v>30</v>
       </c>
-      <c r="F5" s="27" t="n">
+      <c r="F5" s="26" t="n">
         <v>35.9</v>
       </c>
-      <c r="G5" s="27" t="n">
+      <c r="G5" s="26" t="n">
         <v>24</v>
       </c>
-      <c r="H5" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="J5" s="27" t="n">
+      <c r="H5" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="J5" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="L5" s="26" t="n">
         <v>0.6</v>
       </c>
-      <c r="K5" s="27" t="n">
+      <c r="M5" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="L5" s="27" t="n">
+      <c r="N5" s="26" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
-        <v>241</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>242</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="E6" s="27" t="n">
+      <c r="A6" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="E6" s="26" t="n">
         <v>15</v>
       </c>
-      <c r="F6" s="27" t="n">
+      <c r="F6" s="26" t="n">
         <v>17.3</v>
       </c>
-      <c r="G6" s="27" t="n">
+      <c r="G6" s="26" t="n">
         <v>13</v>
       </c>
-      <c r="H6" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="J6" s="27" t="n">
+      <c r="H6" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="J6" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="L6" s="26" t="n">
         <v>0.5</v>
       </c>
-      <c r="K6" s="27" t="n">
+      <c r="M6" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="L6" s="27" t="n">
+      <c r="N6" s="26" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>244</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="E7" s="27" t="n">
+      <c r="A7" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" s="26" t="n">
         <v>14</v>
       </c>
-      <c r="F7" s="27" t="n">
+      <c r="F7" s="26" t="n">
         <v>6.287</v>
       </c>
-      <c r="G7" s="27" t="n">
+      <c r="G7" s="26" t="n">
         <v>4.712</v>
       </c>
-      <c r="H7" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="J7" s="27" t="n">
+      <c r="H7" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="J7" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="L7" s="26" t="n">
         <v>0.4</v>
       </c>
-      <c r="K7" s="27" t="n">
+      <c r="M7" s="26" t="n">
         <v>2</v>
       </c>
-      <c r="L7" s="27" t="n">
+      <c r="N7" s="26" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="C8" s="27" t="s">
+      <c r="A8" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="26" t="n">
+        <v>10.27</v>
+      </c>
+      <c r="F8" s="26" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="G8" s="26" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="H8" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="J8" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="L8" s="26" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M8" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" s="26" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="26" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="F9" s="26" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="G9" s="27" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H9" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="J9" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="L9" s="26" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M9" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="N9" s="26" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="27" t="n">
-        <v>10.27</v>
-      </c>
-      <c r="F8" s="27" t="n">
+      <c r="D10" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="E10" s="26" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="F10" s="26" t="n">
         <v>13.2</v>
       </c>
-      <c r="G8" s="27" t="n">
-        <v>8.8</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="J8" s="27" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K8" s="27" t="n">
+      <c r="G10" s="26" t="n">
+        <v>7.425</v>
+      </c>
+      <c r="H10" s="26" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L8" s="27" t="n">
+      <c r="I10" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="J10" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="L10" s="26" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M10" s="26" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27" t="s">
-        <v>248</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="27" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="F9" s="27" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="G9" s="28" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="J9" s="27" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="K9" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="L9" s="27" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="s">
-        <v>177</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="E10" s="29" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="F10" s="27" t="n">
-        <v>13.2</v>
-      </c>
-      <c r="G10" s="27" t="n">
-        <v>7.425</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="J10" s="27" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="K10" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="L10" s="27" t="n">
+      <c r="N10" s="26" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2217,7 +2331,7 @@
     <row r="24" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2239,16 +2353,18 @@
   </sheetPr>
   <dimension ref="A1:XFD19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="26.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="8" style="2" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="3" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="33.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="33.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16382" min="10" style="2" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2261,6 +2377,8 @@
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -2284,25 +2402,30 @@
       <c r="G2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="XFD2" s="3"/>
+      <c r="H2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="XFC2" s="0"/>
+      <c r="XFD2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="D3" s="16" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="11" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="D3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="F3" s="16" t="b">
         <f aca="false">FALSE()</f>
@@ -2312,30 +2435,44 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="H3" s="16" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="11" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C4" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="16" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="16" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="D4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="F4" s="16" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="11" t="b">
+      <c r="G4" s="16" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="16" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="11" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2345,24 +2482,30 @@
         <v>30</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C5" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="16" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="16" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="D5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="F5" s="16" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G5" s="11" t="b">
+      <c r="G5" s="16" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="16" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="11" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2377,37 +2520,51 @@
       <c r="C6" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="16" t="b">
+      <c r="D6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="16" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E6" s="16" t="b">
+      <c r="G6" s="16" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F6" s="11" t="b">
+      <c r="H6" s="11" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G6" s="11" t="b">
+      <c r="I6" s="11" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="XFC6" s="0"/>
+      <c r="XFD6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14"/>
       <c r="C9" s="13" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2421,7 +2578,7 @@
     <row r="19" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2443,8 +2600,8 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2471,22 +2628,22 @@
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2494,22 +2651,22 @@
         <v>15</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2520,19 +2677,19 @@
         <v>34</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2559,13 +2716,14 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="38.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="2" width="11"/>
   </cols>
   <sheetData>
@@ -2582,76 +2740,76 @@
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E3" s="19" t="n">
         <v>16</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="E4" s="19" t="n">
         <v>16</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>36</v>
@@ -2660,16 +2818,16 @@
         <v>34</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E5" s="19" t="n">
         <v>16</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2702,8 +2860,8 @@
   </sheetPr>
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2714,284 +2872,283 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="29.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="32.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="9" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="13" style="21" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="13" style="20" width="11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16380" min="18" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16381" style="2" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="A1" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="23" t="s">
+      <c r="A2" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>91</v>
       </c>
+      <c r="G2" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>96</v>
+      </c>
       <c r="M2" s="20"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="24" t="s">
+      <c r="A3" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="24" t="n">
+      <c r="D3" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="J3" s="24" t="n">
+      <c r="J3" s="23" t="n">
         <v>250</v>
       </c>
-      <c r="K3" s="24" t="n">
+      <c r="K3" s="23" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="E4" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I4" s="24" t="n">
+      <c r="G4" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="J4" s="24" t="n">
+      <c r="J4" s="23" t="n">
         <v>250</v>
       </c>
-      <c r="K4" s="24" t="n">
+      <c r="K4" s="23" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="I5" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" s="23" t="n">
+        <v>250</v>
+      </c>
+      <c r="K5" s="23" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I5" s="24" t="n">
+      <c r="C6" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="J5" s="24" t="n">
+      <c r="J6" s="23" t="n">
         <v>250</v>
       </c>
-      <c r="K5" s="24" t="n">
+      <c r="K6" s="23" t="n">
         <v>10000</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I6" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="J6" s="24" t="n">
-        <v>250</v>
-      </c>
-      <c r="K6" s="24" t="n">
-        <v>10000</v>
-      </c>
-    </row>
     <row r="7" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="B7" s="24" t="s">
+      <c r="A7" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="G7" s="24" t="s">
+      <c r="C7" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="H7" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I7" s="24" t="n">
+      <c r="F7" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="J7" s="24" t="n">
+      <c r="J7" s="23" t="n">
         <v>300</v>
       </c>
-      <c r="K7" s="24" t="n">
+      <c r="K7" s="23" t="n">
         <v>12000</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="20"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
       <c r="R7" s="20"/>
       <c r="S7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="24" t="s">
+      <c r="A8" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I8" s="24" t="n">
+      <c r="D8" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="J8" s="24" t="n">
+      <c r="J8" s="23" t="n">
         <v>300</v>
       </c>
-      <c r="K8" s="24" t="n">
+      <c r="K8" s="23" t="n">
         <v>12000</v>
       </c>
-      <c r="M8" s="20"/>
     </row>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3034,8 +3191,8 @@
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3048,603 +3205,603 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="A1" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
       <c r="M1" s="2"/>
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="23" t="s">
+      <c r="A2" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="N2" s="20"/>
+    </row>
+    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="I3" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" s="23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="L3" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="I4" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="J4" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="K4" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="L4" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="I5" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="J5" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="K5" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="L5" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="I6" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="J6" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="K6" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="L6" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="I7" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" s="23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="L7" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="I8" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="J8" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="K8" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="L8" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="I9" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" s="23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="L9" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="I10" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="L10" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="I11" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" s="23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="L11" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="I12" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="J12" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="K12" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="L12" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="I13" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="J13" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="K13" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="L13" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="I14" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="J14" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="K14" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="L14" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="I15" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="J15" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="K15" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="L15" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="N2" s="20"/>
-    </row>
-    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="I3" s="24" t="n">
+      <c r="C16" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="I16" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="J3" s="24" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K3" s="24" t="n">
+      <c r="J16" s="23" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K16" s="23" t="n">
         <v>12</v>
       </c>
-      <c r="L3" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="I4" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="J4" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="K4" s="24" t="n">
-        <v>40</v>
-      </c>
-      <c r="L4" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="I5" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="J5" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="K5" s="24" t="n">
-        <v>40</v>
-      </c>
-      <c r="L5" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="I6" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="J6" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="K6" s="24" t="n">
-        <v>40</v>
-      </c>
-      <c r="L6" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="I7" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="J7" s="24" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K7" s="24" t="n">
-        <v>12</v>
-      </c>
-      <c r="L7" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="I8" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="J8" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="K8" s="24" t="n">
-        <v>40</v>
-      </c>
-      <c r="L8" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="I9" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="J9" s="24" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K9" s="24" t="n">
-        <v>12</v>
-      </c>
-      <c r="L9" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="I10" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" s="24" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K10" s="24" t="n">
-        <v>12</v>
-      </c>
-      <c r="L10" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="I11" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="J11" s="24" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K11" s="24" t="n">
-        <v>12</v>
-      </c>
-      <c r="L11" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="I12" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="J12" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="K12" s="24" t="n">
-        <v>40</v>
-      </c>
-      <c r="L12" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="I13" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="J13" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="K13" s="24" t="n">
-        <v>40</v>
-      </c>
-      <c r="L13" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="I14" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="J14" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="K14" s="24" t="n">
-        <v>40</v>
-      </c>
-      <c r="L14" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="I15" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="J15" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="K15" s="24" t="n">
-        <v>40</v>
-      </c>
-      <c r="L15" s="24" t="n">
-        <v>10</v>
-      </c>
-      <c r="M15" s="2"/>
-    </row>
-    <row r="16" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="I16" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="J16" s="24" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K16" s="24" t="n">
-        <v>12</v>
-      </c>
-      <c r="L16" s="24" t="n">
+      <c r="L16" s="23" t="n">
         <v>3</v>
       </c>
       <c r="M16" s="2"/>
@@ -3689,139 +3846,224 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="57.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="20" width="60.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="66.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="48.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="28.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="44.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="29.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="20" width="51.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="20" width="37.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="54.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="20" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="19" style="2" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
+      <c r="A1" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="G2" s="26" t="s">
+      <c r="A2" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>189</v>
       </c>
+      <c r="G2" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="O2" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="P2" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q2" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="R2" s="25" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" s="27" t="n">
+      <c r="A3" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="27" t="n">
+      <c r="E3" s="26" t="n">
         <v>15</v>
       </c>
-      <c r="F3" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="J3" s="27" t="n">
+      <c r="F3" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="H3" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="J3" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="L3" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M3" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="N3" s="26" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="O3" s="26" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="P3" s="26" t="n">
+        <v>250</v>
+      </c>
+      <c r="Q3" s="26" t="n">
         <v>200</v>
       </c>
-      <c r="K3" s="27" t="n">
+      <c r="R3" s="26" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="27" t="n">
+      <c r="A4" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4" s="26" t="n">
         <v>8</v>
       </c>
-      <c r="E4" s="27" t="n">
+      <c r="E4" s="26" t="n">
         <v>12</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="J4" s="27" t="n">
+      <c r="F4" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="H4" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="J4" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="L4" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="N4" s="26" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="O4" s="26" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="P4" s="26" t="n">
+        <v>400</v>
+      </c>
+      <c r="Q4" s="26" t="n">
         <v>350</v>
       </c>
-      <c r="K4" s="27" t="n">
+      <c r="R4" s="26" t="n">
         <v>25</v>
       </c>
     </row>
@@ -3843,7 +4085,7 @@
     <row r="20" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3865,7 +4107,7 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -3878,73 +4120,73 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="A1" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>202</v>
+      <c r="A2" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>214</v>
       </c>
       <c r="G2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>203</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>204</v>
-      </c>
-      <c r="D3" s="27" t="n">
+      <c r="A3" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="D3" s="26" t="n">
         <v>0.4</v>
       </c>
-      <c r="E3" s="27" t="n">
+      <c r="E3" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="F3" s="27" t="n">
+      <c r="F3" s="26" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="D4" s="27" t="n">
+      <c r="A4" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="26" t="n">
         <v>0.6</v>
       </c>
-      <c r="E4" s="27" t="n">
+      <c r="E4" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="F4" s="27" t="n">
+      <c r="F4" s="26" t="n">
         <v>20</v>
       </c>
     </row>
@@ -3985,7 +4227,7 @@
   </sheetPr>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -3999,154 +4241,154 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="A1" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="F2" s="26" t="s">
+      <c r="A2" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="G2" s="26" t="s">
-        <v>212</v>
+      <c r="C2" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>224</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>204</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="E3" s="27" t="n">
+      <c r="A3" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E3" s="26" t="n">
         <v>180</v>
       </c>
-      <c r="F3" s="27" t="n">
+      <c r="F3" s="26" t="n">
         <v>0.1</v>
       </c>
-      <c r="G3" s="27" t="n">
+      <c r="G3" s="26" t="n">
         <v>0.97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>204</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="D4" s="27" t="s">
+      <c r="C4" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" s="26" t="n">
+        <v>180</v>
+      </c>
+      <c r="F4" s="26" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G4" s="26" t="n">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="E4" s="27" t="n">
+      <c r="C5" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="E5" s="26" t="n">
+        <v>270</v>
+      </c>
+      <c r="F5" s="26" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G5" s="26" t="n">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E6" s="26" t="n">
         <v>180</v>
       </c>
-      <c r="F4" s="27" t="n">
+      <c r="F6" s="26" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="26" t="n">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="E7" s="26" t="n">
+        <v>180</v>
+      </c>
+      <c r="F7" s="26" t="n">
         <v>0.05</v>
       </c>
-      <c r="G4" s="27" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
-        <v>219</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>220</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="E5" s="27" t="n">
-        <v>270</v>
-      </c>
-      <c r="F5" s="27" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="G5" s="27" t="n">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="E6" s="27" t="n">
-        <v>180</v>
-      </c>
-      <c r="F6" s="27" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G6" s="27" t="n">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>218</v>
-      </c>
-      <c r="E7" s="27" t="n">
-        <v>180</v>
-      </c>
-      <c r="F7" s="27" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="G7" s="27" t="n">
+      <c r="G7" s="26" t="n">
         <v>0.99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change target trajectories (slower, more dispersion)
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Missions" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="265">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -428,9 +428,6 @@
   </si>
   <si>
     <t xml:space="preserve">MountOrientation [°]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InitialFocal [mm]</t>
   </si>
   <si>
     <t xml:space="preserve">MinFocal [mm]</t>
@@ -1297,9 +1294,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table210" displayName="Table210" ref="A2:K15" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:K15"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table210" displayName="Table210" ref="A2:J15" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:J15"/>
+  <tableColumns count="10">
     <tableColumn id="1" name="HeadID"/>
     <tableColumn id="2" name="HeadPayloadID"/>
     <tableColumn id="3" name="HeadName"/>
@@ -1308,9 +1305,8 @@
     <tableColumn id="6" name="HeadRole"/>
     <tableColumn id="7" name="MountPosition [m]"/>
     <tableColumn id="8" name="MountOrientation [°]"/>
-    <tableColumn id="9" name="InitialFocal [mm]"/>
-    <tableColumn id="10" name="MinFocal [mm]"/>
-    <tableColumn id="11" name="MaxFocal [mm]"/>
+    <tableColumn id="9" name="MinFocal [mm]"/>
+    <tableColumn id="10" name="MaxFocal [mm]"/>
   </tableColumns>
 </table>
 </file>
@@ -1616,7 +1612,7 @@
   </sheetPr>
   <dimension ref="A1:XFD20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1864,8 +1860,8 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1887,7 +1883,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1908,57 +1904,57 @@
         <v>129</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>238</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="J2" s="25" t="s">
         <v>243</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="K2" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="K2" s="25" t="s">
-        <v>245</v>
-      </c>
       <c r="L2" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="M2" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="N2" s="25" t="s">
         <v>213</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="D3" s="26" t="s">
         <v>247</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>248</v>
       </c>
       <c r="E3" s="26" t="n">
         <v>1</v>
@@ -1970,18 +1966,18 @@
         <v>4.712</v>
       </c>
       <c r="H3" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="I3" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="J3" s="26" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="26" t="s">
         <v>249</v>
-      </c>
-      <c r="J3" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K3" s="26" t="s">
-        <v>250</v>
       </c>
       <c r="L3" s="26" t="n">
         <v>0.2</v>
@@ -1995,16 +1991,16 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>251</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>247</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>252</v>
       </c>
       <c r="E4" s="26" t="n">
         <v>10</v>
@@ -2016,18 +2012,18 @@
         <v>8.8</v>
       </c>
       <c r="H4" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="I4" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="J4" s="26" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="26" t="s">
         <v>249</v>
-      </c>
-      <c r="J4" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K4" s="26" t="s">
-        <v>250</v>
       </c>
       <c r="L4" s="26" t="n">
         <v>0.5</v>
@@ -2041,16 +2037,16 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>254</v>
-      </c>
       <c r="C5" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>247</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>248</v>
       </c>
       <c r="E5" s="26" t="n">
         <v>30</v>
@@ -2062,18 +2058,18 @@
         <v>24</v>
       </c>
       <c r="H5" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="I5" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="J5" s="26" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="26" t="s">
         <v>249</v>
-      </c>
-      <c r="J5" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>250</v>
       </c>
       <c r="L5" s="26" t="n">
         <v>0.6</v>
@@ -2087,16 +2083,16 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>256</v>
-      </c>
       <c r="C6" s="26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E6" s="26" t="n">
         <v>15</v>
@@ -2108,18 +2104,18 @@
         <v>13</v>
       </c>
       <c r="H6" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="I6" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="J6" s="26" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="26" t="s">
         <v>249</v>
-      </c>
-      <c r="J6" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K6" s="26" t="s">
-        <v>250</v>
       </c>
       <c r="L6" s="26" t="n">
         <v>0.5</v>
@@ -2133,16 +2129,16 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="B7" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>258</v>
-      </c>
       <c r="C7" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>247</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>248</v>
       </c>
       <c r="E7" s="26" t="n">
         <v>14</v>
@@ -2154,18 +2150,18 @@
         <v>4.712</v>
       </c>
       <c r="H7" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="I7" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="J7" s="26" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="26" t="s">
         <v>249</v>
-      </c>
-      <c r="J7" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K7" s="26" t="s">
-        <v>250</v>
       </c>
       <c r="L7" s="26" t="n">
         <v>0.4</v>
@@ -2179,13 +2175,13 @@
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>259</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="C8" s="26" t="s">
         <v>260</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>261</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>20</v>
@@ -2200,18 +2196,18 @@
         <v>8.8</v>
       </c>
       <c r="H8" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="I8" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="J8" s="26" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="26" t="s">
         <v>249</v>
-      </c>
-      <c r="J8" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K8" s="26" t="s">
-        <v>250</v>
       </c>
       <c r="L8" s="26" t="n">
         <v>0.5</v>
@@ -2225,13 +2221,13 @@
     </row>
     <row r="9" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>262</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="C9" s="26" t="s">
         <v>263</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>264</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>20</v>
@@ -2246,18 +2242,18 @@
         <v>4.7</v>
       </c>
       <c r="H9" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="I9" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="J9" s="26" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="26" t="s">
         <v>249</v>
-      </c>
-      <c r="J9" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>250</v>
       </c>
       <c r="L9" s="26" t="n">
         <v>0.8</v>
@@ -2271,16 +2267,16 @@
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E10" s="26" t="n">
         <v>5.5</v>
@@ -2292,18 +2288,18 @@
         <v>7.425</v>
       </c>
       <c r="H10" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="I10" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="J10" s="26" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="26" t="s">
         <v>249</v>
-      </c>
-      <c r="J10" s="26" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K10" s="26" t="s">
-        <v>250</v>
       </c>
       <c r="L10" s="26" t="n">
         <v>0.8</v>
@@ -2408,8 +2404,8 @@
       <c r="I2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="XFC2" s="0"/>
-      <c r="XFD2" s="0"/>
+      <c r="XFC2" s="3"/>
+      <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
@@ -2542,8 +2538,6 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="XFC6" s="0"/>
-      <c r="XFD6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C7" s="17"/>
@@ -3192,16 +3186,17 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="2" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="20" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="20" width="11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="15" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="2" width="27.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="20" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="15" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="2" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3218,8 +3213,7 @@
       <c r="I1" s="21"/>
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
@@ -3255,521 +3249,480 @@
       <c r="K2" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="L2" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="N2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>99</v>
       </c>
       <c r="C3" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="E3" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="F3" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="G3" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="H3" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="H3" s="23" t="s">
-        <v>143</v>
-      </c>
       <c r="I3" s="23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="K3" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="J3" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K3" s="23" t="n">
-        <v>12</v>
-      </c>
-      <c r="L3" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="M3" s="2"/>
+      <c r="L3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>99</v>
       </c>
       <c r="C4" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="E4" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="F4" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="G4" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="H4" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="H4" s="23" t="s">
-        <v>150</v>
-      </c>
       <c r="I4" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="J4" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="K4" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="J4" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="K4" s="23" t="n">
-        <v>40</v>
-      </c>
-      <c r="L4" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="M4" s="2"/>
+      <c r="L4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>99</v>
       </c>
       <c r="C5" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>153</v>
-      </c>
       <c r="H5" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I5" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="J5" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="K5" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="J5" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="K5" s="23" t="n">
-        <v>40</v>
-      </c>
-      <c r="L5" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="M5" s="2"/>
+      <c r="L5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>99</v>
       </c>
       <c r="C6" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="G6" s="23" t="s">
+      <c r="H6" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="H6" s="23" t="s">
-        <v>157</v>
-      </c>
       <c r="I6" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="J6" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="K6" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="J6" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="K6" s="23" t="n">
-        <v>40</v>
-      </c>
-      <c r="L6" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="M6" s="2"/>
+      <c r="L6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>106</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D7" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="F7" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="G7" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="H7" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="H7" s="23" t="s">
-        <v>143</v>
-      </c>
       <c r="I7" s="23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="K7" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="J7" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K7" s="23" t="n">
-        <v>12</v>
-      </c>
-      <c r="L7" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="M7" s="2"/>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>106</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D8" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="F8" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="G8" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="H8" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="H8" s="23" t="s">
-        <v>150</v>
-      </c>
       <c r="I8" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="J8" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="K8" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="J8" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="K8" s="23" t="n">
-        <v>40</v>
-      </c>
-      <c r="L8" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="M8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>110</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D9" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="F9" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="G9" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="H9" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="H9" s="23" t="s">
-        <v>143</v>
-      </c>
       <c r="I9" s="23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="K9" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="J9" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K9" s="23" t="n">
-        <v>12</v>
-      </c>
-      <c r="L9" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="M9" s="2"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>115</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D10" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="F10" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="G10" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="H10" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="H10" s="23" t="s">
-        <v>143</v>
-      </c>
       <c r="I10" s="23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J10" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="K10" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="J10" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K10" s="23" t="n">
-        <v>12</v>
-      </c>
-      <c r="L10" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="M10" s="2"/>
+      <c r="L10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>120</v>
       </c>
       <c r="C11" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>168</v>
-      </c>
       <c r="I11" s="23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="K11" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="J11" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K11" s="23" t="n">
-        <v>12</v>
-      </c>
-      <c r="L11" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="M11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>120</v>
       </c>
       <c r="C12" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="H12" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D12" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>171</v>
-      </c>
       <c r="I12" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="J12" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="K12" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="J12" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="K12" s="23" t="n">
-        <v>40</v>
-      </c>
-      <c r="L12" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="M12" s="2"/>
+      <c r="L12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>120</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D13" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="F13" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="F13" s="23" t="s">
-        <v>148</v>
-      </c>
       <c r="G13" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I13" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="J13" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="K13" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="J13" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="K13" s="23" t="n">
-        <v>40</v>
-      </c>
-      <c r="L13" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="M13" s="2"/>
+      <c r="L13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>120</v>
       </c>
       <c r="C14" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="H14" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>176</v>
-      </c>
       <c r="I14" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="J14" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="K14" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="J14" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="K14" s="23" t="n">
-        <v>40</v>
-      </c>
-      <c r="L14" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="M14" s="2"/>
+      <c r="L14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>120</v>
       </c>
       <c r="C15" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="G15" s="23" t="s">
+      <c r="H15" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="H15" s="23" t="s">
-        <v>180</v>
-      </c>
       <c r="I15" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="J15" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="K15" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="J15" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="K15" s="23" t="n">
-        <v>40</v>
-      </c>
-      <c r="L15" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="M15" s="2"/>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>123</v>
@@ -3778,34 +3731,32 @@
         <v>34</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E16" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="G16" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="F16" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>183</v>
-      </c>
       <c r="H16" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I16" s="23" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J16" s="23" t="n">
+        <v>12</v>
+      </c>
+      <c r="K16" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="J16" s="23" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K16" s="23" t="n">
-        <v>12</v>
-      </c>
-      <c r="L16" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="20"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3826,7 +3777,7 @@
     <row r="33" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3871,7 +3822,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3896,55 +3847,55 @@
         <v>91</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="J2" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="K2" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="L2" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="M2" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="N2" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="O2" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="P2" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="Q2" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="R2" s="25" t="s">
         <v>200</v>
-      </c>
-      <c r="R2" s="25" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3952,10 +3903,10 @@
         <v>101</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>202</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>203</v>
       </c>
       <c r="D3" s="26" t="n">
         <v>10</v>
@@ -3968,28 +3919,28 @@
         <v>1</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H3" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J3" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L3" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M3" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N3" s="26" t="n">
         <v>4.5</v>
@@ -4012,10 +3963,10 @@
         <v>124</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>208</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>209</v>
       </c>
       <c r="D4" s="26" t="n">
         <v>8</v>
@@ -4028,28 +3979,28 @@
         <v>1</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H4" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I4" s="26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J4" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L4" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M4" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N4" s="26" t="n">
         <v>6.5</v>
@@ -4121,7 +4072,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -4134,31 +4085,31 @@
         <v>128</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>213</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>214</v>
       </c>
       <c r="G2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>215</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>216</v>
       </c>
       <c r="D3" s="26" t="n">
         <v>0.4</v>
@@ -4172,13 +4123,13 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>217</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>218</v>
       </c>
       <c r="D4" s="26" t="n">
         <v>0.6</v>
@@ -4242,7 +4193,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -4253,25 +4204,25 @@
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>211</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>223</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>224</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -4279,16 +4230,16 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="C3" s="26" t="s">
+      <c r="D3" s="26" t="s">
         <v>226</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>227</v>
       </c>
       <c r="E3" s="26" t="n">
         <v>180</v>
@@ -4302,16 +4253,16 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="C4" s="26" t="s">
+      <c r="D4" s="26" t="s">
         <v>229</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>230</v>
       </c>
       <c r="E4" s="26" t="n">
         <v>180</v>
@@ -4325,16 +4276,16 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="C5" s="26" t="s">
+      <c r="D5" s="26" t="s">
         <v>232</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>233</v>
       </c>
       <c r="E5" s="26" t="n">
         <v>270</v>
@@ -4348,16 +4299,16 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C6" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>226</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>227</v>
       </c>
       <c r="E6" s="26" t="n">
         <v>180</v>
@@ -4371,16 +4322,16 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C7" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>229</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>230</v>
       </c>
       <c r="E7" s="26" t="n">
         <v>180</v>

</xml_diff>

<commit_message>
Adjust config for better tracking performance
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Missions" sheetId="1" state="visible" r:id="rId3"/>
@@ -91,727 +91,727 @@
     <t xml:space="preserve">(20.0, 250.0)</t>
   </si>
   <si>
+    <t xml:space="preserve">(720x405)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(480x270)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MISSION01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single-Agent Multi-Camera Wreck Rescue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAP01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUNDLE01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(35.0, 280.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MISSION02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single-Agent Multi-Window Wreck Rescue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MISSION03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Window Demo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUNDLE02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PX4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(30.0, 150.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SimulationName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClockSpeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ScenarioViewPosition [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ScenarioViewOrientation [°]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RecordMetrics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrawRvizMarkers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrawWorldMarkers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableLumen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slow Simple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=-150.0, Y=-150.0, Z=150.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=15.0, Yaw=45.0, Roll=0.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular Simple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular PX4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MapName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RegionType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OriginGeopoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartHour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WindVelocity [m/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(lat=35.9865559, lon=-5.8930106, alt=8.54)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(13/12/2024)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(17:00:00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Vx=5.0, Vy=3.5, Vz=0.8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coastal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GroupID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GroupName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TargetType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TargetCount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GroupPriority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TrajectoryFolder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUP00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fast Human Targets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HighSpeed16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUP01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slow Human Targets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LowSpeed16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUP02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MetaHuman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VeyLowSpeedHighDispersion16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT CONFIGURATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgentID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgentName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HeadPayloadID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TrackingMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DroneModelID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InitialPosition [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InitialOrientation [°]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SafetyRadius [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxAltitude [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BatteryCapacity [mAh]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYLOAD00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MultiWindowTracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRONE00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=15.0, Y=20.0, Z=50.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=0.0, Yaw=0.0, Roll=0.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYLOAD01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=10.0, Y=-20.0, Z=40.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYLOAD02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PriorityHybridTracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=-25.0, Y=10.0, Z=70.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYLOAD03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MultiCameraTracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=-15.0, Y=-20.0, Z=30.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYLOAD04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=-35.0, Y=-20.0, Z=25.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYLOAD05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRONE01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=0.0, Z=0.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HeadID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HeadName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GimbalModelID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CameraModelID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HeadRole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MountPosition [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MountOrientation [°]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MinFocal [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxFocal [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RefFocal [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.1 Central Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIM00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=0.0, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=90, Yaw=90, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.1 Tracking Cam 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIM01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.3, Y=0.0, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=90, Yaw=0, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.1 Tracking Cam 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=0.3, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.1 Tracking Cam 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=-0.3, Y=0.0, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=90, Yaw=180, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.2 Central Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.2 Tracking Cam 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.3 Central Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.4 Central Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 2.1 Central Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=0, Yaw=90, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 2.1 Tracking Cam 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=0, Yaw=0, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 2.1 Tracking Cam 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 2.1 Tracking Cam 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=0, Yaw=180, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 2.1 Tracking Cam 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=-0.3, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=0, Yaw=270, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=0.0, Z=-0.05)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HARDWARE CATALOGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DroneName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DroneType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CruiseSpeed [m/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxSpeed [m/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableBarometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableIMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableGPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableMagnetometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BaseWeight [kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxPayloadWeight [kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HoverPower [W]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CruisePower [W]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoadFactor [W/kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Quadcopter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quadcopter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(PressureSigma=0.0001825, NoiseSigma=3.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(GyroNoise=0.4, AccelNoise=0.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(EphIni=30, EpvIni=40, EphFin=1, EpvFin=2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(NoiseSigma=0.03, ScaleFactor=1.02, NoiseBias=0.05)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DJI S900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hexacopter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GimbalName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkConfigurationID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight [kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IdlePower [W]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ActivePower [W]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Central Gimbal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINKCONFIG00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Tracking Gimbal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINKCONFIG01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GimbalLinkID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JointRange [°]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxAngularSpeed [°/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MotorRiseTime [s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MotorDampingFactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-20.0, 20.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-40.0, 130.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-320.0, 320.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CameraName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CameraType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolution [pix]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DefaultFocal [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SensorWidth [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SensorHeight [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableLensDistortion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LensDistortion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableSensorNoise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SensorNoise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry Pi Camera HQ Lens 2.8 12mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2560x1440)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Strength=0.02, Radius=1.8, Falloff=0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(RandContrib=0.008, RandSize=500, RandSpeed=50000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mavic 2 Pro (Mod. Zoom)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1920x1080)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zenmuse P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zenmuse X5S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry Pi Camera HQ Lens 6 22mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mavic 2 Pro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth</t>
+  </si>
+  <si>
     <t xml:space="preserve">(1280x720)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(640x360)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MISSION01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single-Agent Multi-Camera Wreck Rescue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAP01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUNDLE01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEAM01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(35.0, 280.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MISSION02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single-Agent Multi-Window Wreck Rescue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIM02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEAM02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MISSION03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-Window Demo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIM03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUNDLE02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PX4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(30.0, 150.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SimulationName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClockSpeed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ScenarioViewPosition [m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ScenarioViewOrientation [°]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RecordMetrics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DrawRvizMarkers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DrawWorldMarkers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableLumen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slow Simple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=-150.0, Y=-150.0, Z=150.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=15.0, Yaw=45.0, Roll=0.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIM01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regular Simple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regular PX4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=-250.0, Y=-250.0, Z=150.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MapName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RegionType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OriginGeopoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartHour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WindVelocity [m/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(lat=35.9865559, lon=-5.8930106, alt=8.54)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(13/12/2024)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(17:00:00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Vx=5.0, Vy=3.5, Vz=0.8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coastal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GroupID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GroupName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TargetType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TargetCount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GroupPriority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TrajectoryFolder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GROUP00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fast Human Targets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HighSpeed16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GROUP01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slow Human Targets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LowSpeed16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GROUP02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MetaHuman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VeyLowSpeedHighDispersion16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT CONFIGURATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgentID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgentName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HeadPayloadID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TrackingMode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DroneModelID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InitialPosition [m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InitialOrientation [°]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SafetyRadius [m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxAltitude [m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BatteryCapacity [mAh]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAYLOAD00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MultiWindowTracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DRONE00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=15.0, Y=20.0, Z=50.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=0.0, Yaw=0.0, Roll=0.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAYLOAD01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=10.0, Y=-20.0, Z=40.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAYLOAD02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PriorityHybridTracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=-25.0, Y=10.0, Z=70.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAYLOAD03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MultiCameraTracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=-15.0, Y=-20.0, Z=30.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAYLOAD04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=-35.0, Y=-20.0, Z=25.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAYLOAD05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DRONE01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.0, Y=0.0, Z=0.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HeadID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HeadName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GimbalModelID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CameraModelID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HeadRole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MountPosition [m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MountOrientation [°]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MinFocal [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxFocal [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RefFocal [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.1 Central Cam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIM00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.0, Y=0.0, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=90, Yaw=90, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.1 Tracking Cam 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIM01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.3, Y=0.0, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=90, Yaw=0, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.1 Tracking Cam 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.0, Y=0.3, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.1 Tracking Cam 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=-0.3, Y=0.0, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=90, Yaw=180, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.2 Central Cam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.2 Tracking Cam 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.3 Central Cam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.4 Central Cam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 2.1 Central Cam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=0, Yaw=90, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 2.1 Tracking Cam 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=0, Yaw=0, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 2.1 Tracking Cam 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 2.1 Tracking Cam 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=0, Yaw=180, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 2.1 Tracking Cam 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.0, Y=-0.3, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=0, Yaw=270, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.0, Y=0.0, Z=-0.05)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HARDWARE CATALOGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DroneName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DroneType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CruiseSpeed [m/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxSpeed [m/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableBarometer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barometer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableIMU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableGPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableMagnetometer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magnetometer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BaseWeight [kg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxPayloadWeight [kg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HoverPower [W]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CruisePower [W]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LoadFactor [W/kg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Quadcopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quadcopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(PressureSigma=0.0001825, NoiseSigma=3.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(GyroNoise=0.4, AccelNoise=0.2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(EphIni=30, EpvIni=40, EphFin=1, EpvFin=2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(NoiseSigma=0.03, ScaleFactor=1.02, NoiseBias=0.05)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DJI S900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hexacopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GimbalName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LinkConfigurationID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight [kg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IdlePower [W]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ActivePower [W]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Central Gimbal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINKCONFIG00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Tracking Gimbal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINKCONFIG01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GimbalLinkID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AxisType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JointRange [°]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxAngularSpeed [°/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MotorRiseTime [s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MotorDampingFactor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINK00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-20.0, 20.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINK01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pitch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-40.0, 130.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINK02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-320.0, 320.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINK03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINK04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CameraName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CameraType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolution [pix]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DefaultFocal [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SensorWidth [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SensorHeight [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableLensDistortion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LensDistortion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableSensorNoise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SensorNoise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raspberry Pi Camera HQ Lens 2.8 12mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RGB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2560x1440)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Strength=0.02, Radius=1.8, Falloff=0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(RandContrib=0.008, RandSize=500, RandSpeed=50000)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mavic 2 Pro (Mod. Zoom)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1920x1080)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zenmuse P1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zenmuse X5S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raspberry Pi Camera HQ Lens 6 22mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mavic 2 Pro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth</t>
   </si>
   <si>
     <t xml:space="preserve">CAM06</t>
@@ -1613,7 +1613,7 @@
   <dimension ref="A1:XFD20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1860,8 +1860,8 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1883,7 +1883,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1901,60 +1901,60 @@
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>238</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="J2" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="K2" s="25" t="s">
         <v>243</v>
       </c>
-      <c r="K2" s="25" t="s">
-        <v>244</v>
-      </c>
       <c r="L2" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="M2" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="N2" s="25" t="s">
         <v>212</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="D3" s="26" t="s">
         <v>246</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>247</v>
       </c>
       <c r="E3" s="26" t="n">
         <v>1</v>
@@ -1966,18 +1966,18 @@
         <v>4.712</v>
       </c>
       <c r="H3" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I3" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="J3" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="26" t="s">
         <v>248</v>
-      </c>
-      <c r="J3" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="26" t="s">
-        <v>249</v>
       </c>
       <c r="L3" s="26" t="n">
         <v>0.2</v>
@@ -1991,16 +1991,16 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>250</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>251</v>
       </c>
       <c r="E4" s="26" t="n">
         <v>10</v>
@@ -2012,18 +2012,18 @@
         <v>8.8</v>
       </c>
       <c r="H4" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I4" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="J4" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="26" t="s">
         <v>248</v>
-      </c>
-      <c r="J4" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="26" t="s">
-        <v>249</v>
       </c>
       <c r="L4" s="26" t="n">
         <v>0.5</v>
@@ -2037,16 +2037,16 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>252</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>253</v>
-      </c>
       <c r="C5" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>246</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>247</v>
       </c>
       <c r="E5" s="26" t="n">
         <v>30</v>
@@ -2058,18 +2058,18 @@
         <v>24</v>
       </c>
       <c r="H5" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I5" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="J5" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="26" t="s">
         <v>248</v>
-      </c>
-      <c r="J5" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>249</v>
       </c>
       <c r="L5" s="26" t="n">
         <v>0.6</v>
@@ -2083,16 +2083,16 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="B6" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>255</v>
-      </c>
       <c r="C6" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E6" s="26" t="n">
         <v>15</v>
@@ -2104,18 +2104,18 @@
         <v>13</v>
       </c>
       <c r="H6" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I6" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="J6" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="26" t="s">
         <v>248</v>
-      </c>
-      <c r="J6" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="26" t="s">
-        <v>249</v>
       </c>
       <c r="L6" s="26" t="n">
         <v>0.5</v>
@@ -2129,16 +2129,16 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>257</v>
-      </c>
       <c r="C7" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>246</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>247</v>
       </c>
       <c r="E7" s="26" t="n">
         <v>14</v>
@@ -2150,18 +2150,18 @@
         <v>4.712</v>
       </c>
       <c r="H7" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I7" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="J7" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="26" t="s">
         <v>248</v>
-      </c>
-      <c r="J7" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="26" t="s">
-        <v>249</v>
       </c>
       <c r="L7" s="26" t="n">
         <v>0.4</v>
@@ -2175,16 +2175,16 @@
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>258</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="C8" s="26" t="s">
         <v>259</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="D8" s="26" t="s">
         <v>260</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>20</v>
       </c>
       <c r="E8" s="26" t="n">
         <v>10.27</v>
@@ -2196,18 +2196,18 @@
         <v>8.8</v>
       </c>
       <c r="H8" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I8" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="J8" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="26" t="s">
         <v>248</v>
-      </c>
-      <c r="J8" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="26" t="s">
-        <v>249</v>
       </c>
       <c r="L8" s="26" t="n">
         <v>0.5</v>
@@ -2230,7 +2230,7 @@
         <v>263</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>20</v>
+        <v>260</v>
       </c>
       <c r="E9" s="26" t="n">
         <v>5.5</v>
@@ -2242,18 +2242,18 @@
         <v>4.7</v>
       </c>
       <c r="H9" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I9" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="J9" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="26" t="s">
         <v>248</v>
-      </c>
-      <c r="J9" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>249</v>
       </c>
       <c r="L9" s="26" t="n">
         <v>0.8</v>
@@ -2267,13 +2267,13 @@
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>264</v>
@@ -2288,18 +2288,18 @@
         <v>7.425</v>
       </c>
       <c r="H10" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I10" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="J10" s="26" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="26" t="s">
         <v>248</v>
-      </c>
-      <c r="J10" s="26" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="26" t="s">
-        <v>249</v>
       </c>
       <c r="L10" s="26" t="n">
         <v>0.8</v>
@@ -2350,7 +2350,7 @@
   <dimension ref="A1:XFD19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2517,7 +2517,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>49</v>
@@ -2554,7 +2554,7 @@
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14"/>
       <c r="C9" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2622,22 +2622,22 @@
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2645,22 +2645,22 @@
         <v>15</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="18" t="s">
         <v>65</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2671,19 +2671,19 @@
         <v>34</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="18" t="s">
         <v>65</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2734,76 +2734,76 @@
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="E3" s="19" t="n">
         <v>16</v>
       </c>
       <c r="F3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E4" s="19" t="n">
         <v>16</v>
       </c>
       <c r="F4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>36</v>
@@ -2812,16 +2812,16 @@
         <v>34</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="19" t="n">
         <v>16</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2873,7 +2873,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -2888,37 +2888,37 @@
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="H2" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>95</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>96</v>
       </c>
       <c r="M2" s="20"/>
       <c r="N2" s="20"/>
@@ -2928,28 +2928,28 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="E3" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="F3" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="G3" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="H3" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>103</v>
       </c>
       <c r="I3" s="23" t="n">
         <v>4</v>
@@ -2963,28 +2963,28 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="E4" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>107</v>
-      </c>
       <c r="H4" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I4" s="23" t="n">
         <v>4</v>
@@ -2998,28 +2998,28 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="E5" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="F5" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>112</v>
-      </c>
       <c r="H5" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I5" s="23" t="n">
         <v>4</v>
@@ -3033,28 +3033,28 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="E6" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="F6" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>117</v>
-      </c>
       <c r="H6" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I6" s="23" t="n">
         <v>4</v>
@@ -3068,28 +3068,28 @@
     </row>
     <row r="7" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="E7" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>121</v>
-      </c>
       <c r="H7" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I7" s="23" t="n">
         <v>3</v>
@@ -3111,7 +3111,7 @@
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>31</v>
@@ -3120,19 +3120,19 @@
         <v>34</v>
       </c>
       <c r="D8" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="E8" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" s="23" t="s">
+      <c r="G8" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="G8" s="23" t="s">
-        <v>125</v>
-      </c>
       <c r="H8" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I8" s="23" t="n">
         <v>3</v>
@@ -3185,8 +3185,8 @@
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3201,7 +3201,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -3217,65 +3217,65 @@
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="H2" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>134</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>135</v>
       </c>
       <c r="M2" s="20"/>
       <c r="N2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="23" t="s">
+      <c r="D3" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="E3" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="F3" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="G3" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="H3" s="23" t="s">
         <v>141</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>142</v>
       </c>
       <c r="I3" s="23" t="n">
         <v>0.5</v>
@@ -3290,28 +3290,28 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="23" t="s">
+      <c r="D4" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="E4" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="F4" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="G4" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="H4" s="23" t="s">
         <v>148</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>149</v>
       </c>
       <c r="I4" s="23" t="n">
         <v>8</v>
@@ -3326,28 +3326,28 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" s="23" t="s">
+      <c r="D5" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>152</v>
-      </c>
       <c r="H5" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I5" s="23" t="n">
         <v>8</v>
@@ -3362,28 +3362,28 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="23" t="s">
+      <c r="D6" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="G6" s="23" t="s">
+      <c r="H6" s="23" t="s">
         <v>155</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>156</v>
       </c>
       <c r="I6" s="23" t="n">
         <v>8</v>
@@ -3398,28 +3398,28 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>158</v>
-      </c>
       <c r="D7" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="F7" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="G7" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="H7" s="23" t="s">
         <v>141</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>142</v>
       </c>
       <c r="I7" s="23" t="n">
         <v>0.5</v>
@@ -3434,28 +3434,28 @@
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>160</v>
-      </c>
       <c r="D8" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="F8" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="G8" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="H8" s="23" t="s">
         <v>148</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>149</v>
       </c>
       <c r="I8" s="23" t="n">
         <v>8</v>
@@ -3470,28 +3470,28 @@
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>162</v>
-      </c>
       <c r="D9" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="F9" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="G9" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="H9" s="23" t="s">
         <v>141</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>142</v>
       </c>
       <c r="I9" s="23" t="n">
         <v>0.5</v>
@@ -3506,28 +3506,28 @@
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>164</v>
-      </c>
       <c r="D10" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="F10" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="G10" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="H10" s="23" t="s">
         <v>141</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>142</v>
       </c>
       <c r="I10" s="23" t="n">
         <v>0.5</v>
@@ -3542,28 +3542,28 @@
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="23" t="s">
+      <c r="D11" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" s="23" t="s">
         <v>166</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>167</v>
       </c>
       <c r="I11" s="23" t="n">
         <v>0.5</v>
@@ -3578,28 +3578,28 @@
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" s="23" t="s">
+      <c r="D12" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="H12" s="23" t="s">
         <v>169</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>170</v>
       </c>
       <c r="I12" s="23" t="n">
         <v>8</v>
@@ -3614,28 +3614,28 @@
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>172</v>
-      </c>
       <c r="D13" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="F13" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="23" t="s">
-        <v>147</v>
-      </c>
       <c r="G13" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I13" s="23" t="n">
         <v>8</v>
@@ -3650,28 +3650,28 @@
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="B14" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="C14" s="23" t="s">
+      <c r="D14" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="H14" s="23" t="s">
         <v>174</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>175</v>
       </c>
       <c r="I14" s="23" t="n">
         <v>8</v>
@@ -3686,28 +3686,28 @@
     </row>
     <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="23" t="s">
+      <c r="D15" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="G15" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="G15" s="23" t="s">
+      <c r="H15" s="23" t="s">
         <v>178</v>
-      </c>
-      <c r="H15" s="23" t="s">
-        <v>179</v>
       </c>
       <c r="I15" s="23" t="n">
         <v>8</v>
@@ -3722,28 +3722,28 @@
     </row>
     <row r="16" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" s="23" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E16" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="G16" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="F16" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>182</v>
-      </c>
       <c r="H16" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I16" s="23" t="n">
         <v>0.1</v>
@@ -3822,7 +3822,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3844,69 +3844,69 @@
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="J2" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="K2" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="L2" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="M2" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="N2" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="O2" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="P2" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="Q2" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="R2" s="25" t="s">
         <v>199</v>
-      </c>
-      <c r="R2" s="25" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>201</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>202</v>
       </c>
       <c r="D3" s="26" t="n">
         <v>10</v>
@@ -3919,28 +3919,28 @@
         <v>1</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H3" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J3" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L3" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M3" s="26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N3" s="26" t="n">
         <v>4.5</v>
@@ -3960,13 +3960,13 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>207</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>208</v>
       </c>
       <c r="D4" s="26" t="n">
         <v>8</v>
@@ -3979,28 +3979,28 @@
         <v>1</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H4" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I4" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J4" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L4" s="26" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M4" s="26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N4" s="26" t="n">
         <v>6.5</v>
@@ -4072,7 +4072,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -4082,34 +4082,34 @@
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>212</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>213</v>
       </c>
       <c r="G2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>214</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>215</v>
       </c>
       <c r="D3" s="26" t="n">
         <v>0.4</v>
@@ -4123,13 +4123,13 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>216</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>217</v>
       </c>
       <c r="D4" s="26" t="n">
         <v>0.6</v>
@@ -4193,7 +4193,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -4204,25 +4204,25 @@
     </row>
     <row r="2" s="8" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>222</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>223</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -4230,16 +4230,16 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>215</v>
-      </c>
-      <c r="C3" s="26" t="s">
+      <c r="D3" s="26" t="s">
         <v>225</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>226</v>
       </c>
       <c r="E3" s="26" t="n">
         <v>180</v>
@@ -4253,16 +4253,16 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>215</v>
-      </c>
-      <c r="C4" s="26" t="s">
+      <c r="D4" s="26" t="s">
         <v>228</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>229</v>
       </c>
       <c r="E4" s="26" t="n">
         <v>180</v>
@@ -4276,16 +4276,16 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="C5" s="26" t="s">
+      <c r="D5" s="26" t="s">
         <v>231</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>232</v>
       </c>
       <c r="E5" s="26" t="n">
         <v>270</v>
@@ -4299,16 +4299,16 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C6" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>225</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>226</v>
       </c>
       <c r="E6" s="26" t="n">
         <v>180</v>
@@ -4322,16 +4322,16 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C7" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>228</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>229</v>
       </c>
       <c r="E7" s="26" t="n">
         <v>180</v>

</xml_diff>

<commit_message>
Create and update various README.md
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Missions" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="267">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -232,7 +232,7 @@
     <t xml:space="preserve">Coastal</t>
   </si>
   <si>
-    <t xml:space="preserve">(17:30:00)</t>
+    <t xml:space="preserve">(16:30:00)</t>
   </si>
   <si>
     <t xml:space="preserve">GroupID</t>
@@ -827,6 +827,9 @@
   </si>
   <si>
     <t xml:space="preserve">(7680x4320)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(RandContrib=0.001, RandSize=100, RandSpeed=50000)</t>
   </si>
 </sst>
 </file>
@@ -1863,8 +1866,8 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2302,7 +2305,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="26" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="L10" s="26" t="n">
         <v>0.8</v>
@@ -2597,8 +2600,8 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3253,7 +3256,7 @@
         <v>135</v>
       </c>
       <c r="M2" s="20"/>
-      <c r="N2" s="0"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
@@ -3759,7 +3762,6 @@
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="20"/>
-      <c r="N16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Change window config structure
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Mission" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="196">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -337,7 +337,7 @@
     <t xml:space="preserve">HEAD01</t>
   </si>
   <si>
-    <t xml:space="preserve">Multi-Camera Tracking Cam 1</t>
+    <t xml:space="preserve">Multi-Camera Tracking Head 1</t>
   </si>
   <si>
     <t xml:space="preserve">CAM01</t>
@@ -349,7 +349,7 @@
     <t xml:space="preserve">HEAD02</t>
   </si>
   <si>
-    <t xml:space="preserve">Multi-Camera Tracking Cam 2</t>
+    <t xml:space="preserve">Multi-Camera Tracking Head 2</t>
   </si>
   <si>
     <t xml:space="preserve">(X=0.0, Y=0.3, Z=-0.15)</t>
@@ -361,7 +361,7 @@
     <t xml:space="preserve">HEAD03</t>
   </si>
   <si>
-    <t xml:space="preserve">Multi-Camera Tracking Cam 3</t>
+    <t xml:space="preserve">Multi-Camera Tracking Head 3</t>
   </si>
   <si>
     <t xml:space="preserve">(X=-0.3, Y=0.0, Z=-0.15)</t>
@@ -373,7 +373,7 @@
     <t xml:space="preserve">HEAD04</t>
   </si>
   <si>
-    <t xml:space="preserve">Multi-Camera Tracking Cam 4</t>
+    <t xml:space="preserve">Multi-Camera Tracking Head 4</t>
   </si>
   <si>
     <t xml:space="preserve">(X=0.0, Y=-0.3, Z=-0.15)</t>
@@ -385,7 +385,25 @@
     <t xml:space="preserve">HEAD05</t>
   </si>
   <si>
-    <t xml:space="preserve">Multi-Camera Central Cam</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Multi-Camera Central </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Head</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">CAM02</t>
@@ -397,12 +415,33 @@
     <t xml:space="preserve">HEAD06</t>
   </si>
   <si>
-    <t xml:space="preserve">Multi-Window Central Cam</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Multi-Window Central </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Head</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">CAM03</t>
   </si>
   <si>
+    <t xml:space="preserve">Resolution [pix]</t>
+  </si>
+  <si>
     <t xml:space="preserve">MinLambda</t>
   </si>
   <si>
@@ -412,31 +451,37 @@
     <t xml:space="preserve">RefLambda</t>
   </si>
   <si>
-    <t xml:space="preserve">Resolution [pix]</t>
-  </si>
-  <si>
     <t xml:space="preserve">WINDOW00</t>
   </si>
   <si>
+    <t xml:space="preserve">Multi-Window Central Window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1280x720)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINDOW01</t>
+  </si>
+  <si>
     <t xml:space="preserve">Multi-Window Tracking Window 1</t>
   </si>
   <si>
     <t xml:space="preserve">(240x135)</t>
   </si>
   <si>
-    <t xml:space="preserve">WINDOW01</t>
+    <t xml:space="preserve">WINDOW02</t>
   </si>
   <si>
     <t xml:space="preserve">Multi-Window Tracking Window 2</t>
   </si>
   <si>
-    <t xml:space="preserve">WINDOW02</t>
+    <t xml:space="preserve">WINDOW03</t>
   </si>
   <si>
     <t xml:space="preserve">Multi-Window Tracking Window 3</t>
   </si>
   <si>
-    <t xml:space="preserve">WINDOW03</t>
+    <t xml:space="preserve">WINDOW04</t>
   </si>
   <si>
     <t xml:space="preserve">Multi-Window Tracking Window 4</t>
@@ -572,9 +617,6 @@
   </si>
   <si>
     <t xml:space="preserve">RGB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1280x720)</t>
   </si>
   <si>
     <t xml:space="preserve">(13.2x8.8)</t>
@@ -622,7 +664,7 @@
     <numFmt numFmtId="165" formatCode="h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -690,6 +732,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -777,7 +825,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -855,6 +903,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1061,15 +1113,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table210_2" displayName="Table210_2" ref="A2:F6" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:F6"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table210_2" displayName="Table210_2" ref="A2:H7" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:H7"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="WindowSetID"/>
-    <tableColumn id="4" name="MinLambda"/>
-    <tableColumn id="5" name="MaxLambda"/>
-    <tableColumn id="6" name="RefLambda"/>
+    <tableColumn id="4" name="Role"/>
+    <tableColumn id="5" name="Resolution [pix]"/>
+    <tableColumn id="6" name="MinLambda"/>
+    <tableColumn id="7" name="MaxLambda"/>
+    <tableColumn id="8" name="RefLambda"/>
   </tableColumns>
 </table>
 </file>
@@ -1667,218 +1721,218 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
+      <c r="A1" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="H2" s="21" t="s">
+      <c r="D2" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="F2" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="J2" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>169</v>
+      <c r="G2" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>172</v>
       </c>
       <c r="XFC2" s="3"/>
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="E3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="F3" s="22" t="b">
+      <c r="C3" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G3" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="H3" s="22" t="b">
+      <c r="G3" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="H3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="J3" s="23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="L3" s="23" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="J3" s="22" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K3" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="L3" s="22" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="F4" s="22" t="b">
+      <c r="F4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G4" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="H4" s="22" t="b">
+      <c r="G4" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="H4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I4" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="J4" s="22" t="n">
+      <c r="I4" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="J4" s="23" t="n">
         <v>0.5</v>
       </c>
-      <c r="K4" s="22" t="n">
+      <c r="K4" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="L4" s="22" t="n">
+      <c r="L4" s="23" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="E5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="F5" s="22" t="b">
+      <c r="C5" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="F5" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G5" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="H5" s="22" t="b">
+      <c r="G5" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="H5" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I5" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="J5" s="22" t="n">
+      <c r="I5" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="J5" s="23" t="n">
         <v>0.2</v>
       </c>
-      <c r="K5" s="22" t="n">
+      <c r="K5" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="L5" s="22" t="n">
+      <c r="L5" s="23" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="E6" s="22" t="s">
+      <c r="B6" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="F6" s="22" t="b">
+      <c r="C6" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G6" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="H6" s="22" t="b">
+      <c r="G6" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="H6" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I6" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="J6" s="22" t="n">
+      <c r="I6" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="J6" s="23" t="n">
         <v>0.8</v>
       </c>
-      <c r="K6" s="22" t="n">
+      <c r="K6" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="L6" s="22" t="n">
+      <c r="L6" s="23" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2013,7 +2067,7 @@
   </sheetPr>
   <dimension ref="A1:BM9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -2682,7 +2736,7 @@
   <dimension ref="A1:XFD26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3045,20 +3099,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:XFD23"/>
+  <dimension ref="A1:XFD21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="38.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="12" width="27.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16375" min="8" style="2" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16376" style="3" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="12" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="12" width="27.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16376" min="9" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16377" style="3" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3071,6 +3128,7 @@
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
@@ -3083,18 +3141,20 @@
         <v>56</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="XEV2" s="3"/>
       <c r="XEW2" s="3"/>
       <c r="XEX2" s="3"/>
       <c r="XEY2" s="3"/>
@@ -3102,7 +3162,7 @@
       <c r="XFA2" s="3"/>
       <c r="XFB2" s="3"/>
       <c r="XFC2" s="3"/>
-      <c r="XFD2" s="3"/>
+      <c r="XFD2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
@@ -3114,18 +3174,28 @@
       <c r="C3" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="19" t="n">
+      <c r="D3" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="19" t="n">
         <v>0.167</v>
       </c>
-      <c r="E3" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="19" t="n">
-        <v>0.583</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>130</v>
-      </c>
+      <c r="G3" s="20" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="H3" s="20" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="XEW3" s="0"/>
+      <c r="XEX3" s="0"/>
+      <c r="XEY3" s="0"/>
+      <c r="XEZ3" s="0"/>
+      <c r="XFA3" s="0"/>
+      <c r="XFB3" s="0"/>
+      <c r="XFC3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
@@ -3137,66 +3207,100 @@
       <c r="C4" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="19" t="n">
+      <c r="D4" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" s="19" t="n">
         <v>0.167</v>
       </c>
-      <c r="E4" s="19" t="n">
+      <c r="G4" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="19" t="n">
+      <c r="H4" s="19" t="n">
         <v>0.583</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="19" t="n">
+      <c r="D5" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="19" t="n">
         <v>0.167</v>
       </c>
-      <c r="E5" s="19" t="n">
+      <c r="G5" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="19" t="n">
+      <c r="H5" s="19" t="n">
         <v>0.583</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="19" t="n">
+      <c r="D6" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="19" t="n">
         <v>0.167</v>
       </c>
-      <c r="E6" s="19" t="n">
+      <c r="G6" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="19" t="n">
+      <c r="H6" s="19" t="n">
         <v>0.583</v>
       </c>
-      <c r="G6" s="19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="19" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="G7" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="19" t="n">
+        <v>0.583</v>
+      </c>
+    </row>
     <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3211,11 +3315,9 @@
     <row r="19" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3259,200 +3361,200 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
+      <c r="A1" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="G2" s="21" t="s">
+      <c r="D2" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="E2" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="F2" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="G2" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="H2" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="I2" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="J2" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="K2" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="L2" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="M2" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="N2" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="R2" s="21" t="s">
+      <c r="O2" s="22" t="s">
         <v>152</v>
       </c>
+      <c r="P2" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="R2" s="22" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" s="22" t="n">
+      <c r="B3" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="22" t="n">
+      <c r="E3" s="23" t="n">
         <v>15</v>
       </c>
-      <c r="F3" s="22" t="b">
+      <c r="F3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G3" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="H3" s="22" t="b">
+      <c r="G3" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="H3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I3" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="J3" s="22" t="b">
+      <c r="I3" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="J3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K3" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="L3" s="22" t="b">
+      <c r="K3" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="L3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M3" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="N3" s="22" t="n">
+      <c r="M3" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="N3" s="23" t="n">
         <v>4.5</v>
       </c>
-      <c r="O3" s="22" t="n">
+      <c r="O3" s="23" t="n">
         <v>1.5</v>
       </c>
-      <c r="P3" s="22" t="n">
+      <c r="P3" s="23" t="n">
         <v>250</v>
       </c>
-      <c r="Q3" s="22" t="n">
+      <c r="Q3" s="23" t="n">
         <v>200</v>
       </c>
-      <c r="R3" s="22" t="n">
+      <c r="R3" s="23" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="D4" s="22" t="n">
+      <c r="B4" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="E4" s="22" t="n">
+      <c r="E4" s="23" t="n">
         <v>12</v>
       </c>
-      <c r="F4" s="22" t="b">
+      <c r="F4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G4" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="H4" s="22" t="b">
+      <c r="G4" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I4" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="J4" s="22" t="b">
+      <c r="I4" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="J4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K4" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="L4" s="22" t="b">
+      <c r="K4" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="L4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M4" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="N4" s="22" t="n">
+      <c r="M4" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="N4" s="23" t="n">
         <v>6.5</v>
       </c>
-      <c r="O4" s="22" t="n">
+      <c r="O4" s="23" t="n">
         <v>2.5</v>
       </c>
-      <c r="P4" s="22" t="n">
+      <c r="P4" s="23" t="n">
         <v>400</v>
       </c>
-      <c r="Q4" s="22" t="n">
+      <c r="Q4" s="23" t="n">
         <v>350</v>
       </c>
-      <c r="R4" s="22" t="n">
+      <c r="R4" s="23" t="n">
         <v>25</v>
       </c>
     </row>
@@ -3514,92 +3616,92 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="A1" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="F2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="D2" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="E2" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="F2" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="G2" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="H2" s="22" t="s">
         <v>169</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>172</v>
       </c>
       <c r="L2" s="12"/>
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" s="22" t="b">
+      <c r="B3" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" s="22" t="b">
+      <c r="D3" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F3" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="22" t="b">
+      <c r="F3" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H3" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="I3" s="22" t="n">
+      <c r="H3" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="I3" s="23" t="n">
         <v>0.4</v>
       </c>
-      <c r="J3" s="22" t="n">
+      <c r="J3" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="K3" s="22" t="n">
+      <c r="K3" s="23" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solve central cost parameters issues
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Mission" sheetId="1" state="visible" r:id="rId3"/>
@@ -2526,8 +2526,8 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2690,7 +2690,7 @@
   <dimension ref="A1:XFD26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3009,7 +3009,7 @@
         <v>12</v>
       </c>
       <c r="K9" s="19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="12"/>
@@ -3055,7 +3055,7 @@
   </sheetPr>
   <dimension ref="A1:XFD21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update drone model sensors
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Mission" sheetId="1" state="visible" r:id="rId3"/>
@@ -505,16 +505,16 @@
     <t xml:space="preserve">Quadcopter</t>
   </si>
   <si>
-    <t xml:space="preserve">(PressureSigma=0.0001825, NoiseSigma=3.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(GyroNoise=0.4, AccelNoise=0.2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(EphIni=30, EpvIni=40, EphFin=1, EpvFin=2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(NoiseSigma=0.03, ScaleFactor=1.02, NoiseBias=0.05)</t>
+    <t xml:space="preserve">(WhiteNoiseSigma=2.7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(AngularWhiteNoiseSigma=0.3, VelocityWhiteNoiseSigma=0.24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(EphIni=25, EpvIni=25, EphFin=0.1, EpvFin=0.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(WhiteNoiseSigma=0.005, WhiteNoiseBias=0)</t>
   </si>
   <si>
     <t xml:space="preserve">DJI S900</t>
@@ -1650,8 +1650,8 @@
   </sheetPr>
   <dimension ref="A1:XFD20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1666,8 +1666,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="30.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="26.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="12" style="2" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16382" min="16382" style="0" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="3" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="3" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1719,7 +1718,7 @@
       <c r="K2" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="XFB2" s="0"/>
+      <c r="XFB2" s="3"/>
       <c r="XFC2" s="3"/>
       <c r="XFD2" s="3"/>
     </row>
@@ -1830,7 +1829,6 @@
       <c r="K5" s="22" t="n">
         <v>5</v>
       </c>
-      <c r="XFB5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
@@ -3263,17 +3261,17 @@
   </sheetPr>
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="34.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="48.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="35.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="28.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="44.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="64.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="29.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="12" width="51.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="12" width="37.81"/>

</xml_diff>

<commit_message>
Implement ellipsoid method to agent positioning
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Mission" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="197">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -49,7 +49,10 @@
     <t xml:space="preserve">AgentTeamID</t>
   </si>
   <si>
-    <t xml:space="preserve">AltitudeConstraint [m]</t>
+    <t xml:space="preserve">HorizontalConstraint [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VerticalConstraint [m]</t>
   </si>
   <si>
     <t xml:space="preserve">Autopilot</t>
@@ -74,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">TEAM00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-150.0, 150.0)</t>
   </si>
   <si>
     <t xml:space="preserve">(30.0, 150.0)</t>
@@ -1031,16 +1037,17 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table72" displayName="Table72" ref="A2:G3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:G3"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table72" displayName="Table72" ref="A2:H3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:H3"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="ID2"/>
     <tableColumn id="2" name="ID"/>
     <tableColumn id="3" name="Name"/>
     <tableColumn id="4" name="EnvironmentID"/>
     <tableColumn id="5" name="TargetGroupID"/>
     <tableColumn id="6" name="AgentTeamID"/>
-    <tableColumn id="7" name="AltitudeConstraint [m]"/>
+    <tableColumn id="7" name="HorizontalConstraint [m]"/>
+    <tableColumn id="8" name="VerticalConstraint [m]"/>
   </tableColumns>
 </table>
 </file>
@@ -1363,8 +1370,8 @@
   </sheetPr>
   <dimension ref="A1:XFD19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1373,10 +1380,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="54.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="2" width="26.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="2" width="20.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="11" style="2" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="3" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="29.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="30.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="2" width="20.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16382" min="12" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="3" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1392,6 +1401,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5"/>
@@ -1416,76 +1426,83 @@
       <c r="H2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="XFB2" s="3"/>
+      <c r="K2" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="XFC2" s="3"/>
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8"/>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="I3" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="J3" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="12"/>
+      <c r="K4" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
@@ -1530,39 +1547,42 @@
       <c r="BA4" s="12"/>
       <c r="BB4" s="12"/>
       <c r="BC4" s="12"/>
+      <c r="BD4" s="12"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="J5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
@@ -1607,12 +1627,15 @@
       <c r="BA5" s="12"/>
       <c r="BB5" s="12"/>
       <c r="BC5" s="12"/>
+      <c r="BD5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1628,7 +1651,7 @@
     <row r="19" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1671,7 +1694,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -1692,31 +1715,31 @@
         <v>2</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="XFB2" s="3"/>
       <c r="XFC2" s="3"/>
@@ -1724,29 +1747,29 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="I3" s="22" t="n">
         <v>0.5</v>
@@ -1760,29 +1783,29 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B4" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>186</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>184</v>
       </c>
       <c r="G4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="I4" s="22" t="n">
         <v>0.5</v>
@@ -1796,29 +1819,29 @@
     </row>
     <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G5" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="I5" s="22" t="n">
         <v>0.2</v>
@@ -1832,29 +1855,29 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G6" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="I6" s="22" t="n">
         <v>0.8</v>
@@ -1939,38 +1962,38 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="D4" s="15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2033,63 +2056,63 @@
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="BM2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E3" s="16" t="n">
         <v>16</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E4" s="16" t="n">
         <v>16</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -2152,25 +2175,25 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="E5" s="16" t="n">
         <v>8</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -2282,7 +2305,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -2307,31 +2330,31 @@
         <v>5</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N2" s="12"/>
       <c r="O2" s="12"/>
@@ -2341,31 +2364,31 @@
     </row>
     <row r="3" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J3" s="19" t="n">
         <v>300</v>
@@ -2387,31 +2410,31 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="I4" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>70</v>
       </c>
       <c r="J4" s="19" t="n">
         <v>300</v>
@@ -2425,31 +2448,31 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>74</v>
-      </c>
       <c r="H5" s="19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J5" s="19" t="n">
         <v>300</v>
@@ -2522,7 +2545,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -2538,16 +2561,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
@@ -2563,13 +2586,13 @@
     </row>
     <row r="3" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D3" s="19" t="n">
         <v>0.2</v>
@@ -2594,13 +2617,13 @@
     </row>
     <row r="4" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D4" s="19" t="n">
         <v>0.2</v>
@@ -2684,7 +2707,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -2706,31 +2729,31 @@
         <v>2</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="3"/>
@@ -2738,28 +2761,28 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I3" s="19" t="n">
         <v>8</v>
@@ -2774,28 +2797,28 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>102</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>100</v>
       </c>
       <c r="I4" s="19" t="n">
         <v>8</v>
@@ -2810,28 +2833,28 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>103</v>
-      </c>
       <c r="F5" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I5" s="19" t="n">
         <v>8</v>
@@ -2846,28 +2869,28 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I6" s="19" t="n">
         <v>8</v>
@@ -2882,28 +2905,28 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I7" s="19" t="n">
         <v>8</v>
@@ -2918,28 +2941,28 @@
     </row>
     <row r="8" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I8" s="19" t="n">
         <v>1</v>
@@ -2955,28 +2978,28 @@
     </row>
     <row r="9" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>120</v>
-      </c>
       <c r="G9" s="19" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I9" s="19" t="n">
         <v>1</v>
@@ -3049,7 +3072,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -3067,22 +3090,22 @@
         <v>2</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="XEW2" s="3"/>
       <c r="XEX2" s="3"/>
@@ -3095,19 +3118,19 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F3" s="19" t="n">
         <v>0.167</v>
@@ -3121,19 +3144,19 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F4" s="19" t="n">
         <v>0.167</v>
@@ -3147,19 +3170,19 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="19" t="s">
         <v>135</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>133</v>
       </c>
       <c r="F5" s="19" t="n">
         <v>0.167</v>
@@ -3173,19 +3196,19 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F6" s="19" t="n">
         <v>0.167</v>
@@ -3199,19 +3222,19 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F7" s="19" t="n">
         <v>0.167</v>
@@ -3261,7 +3284,7 @@
   </sheetPr>
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -3284,7 +3307,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -3312,63 +3335,63 @@
         <v>2</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="Q2" s="21" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="R2" s="21" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D3" s="22" t="n">
         <v>10</v>
@@ -3381,28 +3404,28 @@
         <v>1</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="J3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="L3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="N3" s="22" t="n">
         <v>4.5</v>
@@ -3422,13 +3445,13 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D4" s="22" t="n">
         <v>8</v>
@@ -3441,28 +3464,28 @@
         <v>1</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="J4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="L4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M4" s="22" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="N4" s="22" t="n">
         <v>6.5</v>
@@ -3539,7 +3562,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -3560,62 +3583,62 @@
         <v>2</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="L2" s="12"/>
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="G3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I3" s="22" t="n">
         <v>0.4</v>

</xml_diff>

<commit_message>
Upgrade sub-optimal combinatorial implementation
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -2685,8 +2685,8 @@
   </sheetPr>
   <dimension ref="A1:XFD26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Publish DebugSolver message for solver comparison
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Mission" sheetId="1" state="visible" r:id="rId3"/>
@@ -94,28 +94,28 @@
     <t xml:space="preserve">(14:30:00)</t>
   </si>
   <si>
+    <t xml:space="preserve">MISSION01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coastal SAR Mission (Multi-Camera-Tracking)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENVIRONMENT01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUP02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PX4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(16:30:00)</t>
+  </si>
+  <si>
     <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MISSION01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coastal SAR Mission (Multi-Camera-Tracking)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENVIRONMENT01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GROUP02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEAM01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PX4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(16:30:00)</t>
   </si>
   <si>
     <t xml:space="preserve">MISSION02</t>
@@ -625,7 +625,7 @@
     <numFmt numFmtId="165" formatCode="h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -693,6 +693,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -780,7 +787,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -831,6 +838,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -894,7 +905,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
+          <fgColor rgb="FFDAE3F3"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -902,7 +913,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFDAE3F3"/>
+          <fgColor rgb="FF000000"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1365,7 +1376,7 @@
   <dimension ref="A1:XFD19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1466,23 +1477,21 @@
       </c>
     </row>
     <row r="4" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="10" t="s">
         <v>25</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>16</v>
@@ -1491,13 +1500,13 @@
         <v>17</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
@@ -1546,7 +1555,9 @@
       <c r="BD4" s="12"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8"/>
+      <c r="A5" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="B5" s="9" t="s">
         <v>29</v>
       </c>
@@ -1554,10 +1565,10 @@
         <v>30</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>31</v>
@@ -1569,13 +1580,13 @@
         <v>17</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
@@ -1624,12 +1635,12 @@
       <c r="BD5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1667,7 +1678,7 @@
   </sheetPr>
   <dimension ref="A1:XFD20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1687,52 +1698,52 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="22" t="s">
         <v>174</v>
       </c>
       <c r="XFB2" s="3"/>
@@ -1740,146 +1751,146 @@
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="G3" s="22" t="b">
+      <c r="G3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="I3" s="22" t="n">
+      <c r="I3" s="23" t="n">
         <v>0.5</v>
       </c>
-      <c r="J3" s="22" t="n">
+      <c r="J3" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="K3" s="22" t="n">
+      <c r="K3" s="23" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="G4" s="22" t="b">
+      <c r="G4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="I4" s="22" t="n">
+      <c r="I4" s="23" t="n">
         <v>0.5</v>
       </c>
-      <c r="J4" s="22" t="n">
+      <c r="J4" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="K4" s="22" t="n">
+      <c r="K4" s="23" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="G5" s="22" t="b">
+      <c r="G5" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="I5" s="22" t="n">
+      <c r="I5" s="23" t="n">
         <v>0.2</v>
       </c>
-      <c r="J5" s="22" t="n">
+      <c r="J5" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="K5" s="22" t="n">
+      <c r="K5" s="23" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="G6" s="22" t="b">
+      <c r="G6" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="I6" s="22" t="n">
+      <c r="I6" s="23" t="n">
         <v>0.8</v>
       </c>
-      <c r="J6" s="22" t="n">
+      <c r="J6" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="K6" s="22" t="n">
+      <c r="K6" s="23" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1938,12 +1949,12 @@
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
       <c r="E1" s="12"/>
       <c r="XFB1" s="3"/>
       <c r="XFC1" s="3"/>
@@ -1972,13 +1983,13 @@
       <c r="C3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="16" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>37</v>
@@ -1986,7 +1997,7 @@
       <c r="C4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2029,15 +2040,15 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -2076,7 +2087,7 @@
       <c r="D3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="16" t="n">
+      <c r="E3" s="17" t="n">
         <v>16</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -2099,7 +2110,7 @@
       <c r="D4" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="16" t="n">
+      <c r="E4" s="17" t="n">
         <v>16</v>
       </c>
       <c r="F4" s="9" t="s">
@@ -2175,12 +2186,12 @@
         <v>53</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="16" t="n">
+      <c r="E5" s="17" t="n">
         <v>8</v>
       </c>
       <c r="F5" s="9" t="s">
@@ -2276,7 +2287,7 @@
   </sheetPr>
   <dimension ref="A1:XFD22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -2298,56 +2309,56 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="19" t="s">
         <v>64</v>
       </c>
       <c r="N2" s="12"/>
@@ -2357,40 +2368,40 @@
       <c r="R2" s="12"/>
     </row>
     <row r="3" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="19" t="n">
+      <c r="J3" s="20" t="n">
         <v>300</v>
       </c>
-      <c r="K3" s="19" t="n">
+      <c r="K3" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="L3" s="19" t="n">
+      <c r="L3" s="20" t="n">
         <v>12000</v>
       </c>
       <c r="M3" s="2"/>
@@ -2406,78 +2417,78 @@
       <c r="XFD3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="19" t="s">
+      <c r="C4" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="J4" s="19" t="n">
+      <c r="J4" s="20" t="n">
         <v>300</v>
       </c>
-      <c r="K4" s="19" t="n">
+      <c r="K4" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="L4" s="19" t="n">
+      <c r="L4" s="20" t="n">
         <v>12000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="19" t="n">
+      <c r="J5" s="20" t="n">
         <v>300</v>
       </c>
-      <c r="K5" s="19" t="n">
+      <c r="K5" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="L5" s="19" t="n">
+      <c r="L5" s="20" t="n">
         <v>12000</v>
       </c>
     </row>
@@ -2541,32 +2552,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="19" t="s">
         <v>85</v>
       </c>
       <c r="H2" s="12"/>
@@ -2582,22 +2593,22 @@
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="19" t="n">
+      <c r="D3" s="20" t="n">
         <v>0.2</v>
       </c>
-      <c r="E3" s="19" t="n">
+      <c r="E3" s="20" t="n">
         <v>0.9</v>
       </c>
-      <c r="F3" s="19" t="n">
+      <c r="F3" s="20" t="n">
         <v>0.6</v>
       </c>
       <c r="G3" s="2"/>
@@ -2613,22 +2624,22 @@
       <c r="XEX3" s="2"/>
     </row>
     <row r="4" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="19" t="n">
+      <c r="D4" s="20" t="n">
         <v>0.2</v>
       </c>
-      <c r="E4" s="19" t="n">
+      <c r="E4" s="20" t="n">
         <v>0.9</v>
       </c>
-      <c r="F4" s="19" t="n">
+      <c r="F4" s="20" t="n">
         <v>0.6</v>
       </c>
       <c r="G4" s="2"/>
@@ -2685,7 +2696,7 @@
   </sheetPr>
   <dimension ref="A1:XFD26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2703,53 +2714,53 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
       <c r="L1" s="2"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="19" t="s">
         <v>95</v>
       </c>
       <c r="M2" s="12"/>
@@ -2757,254 +2768,254 @@
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="I3" s="19" t="n">
+      <c r="I3" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="J3" s="19" t="n">
+      <c r="J3" s="20" t="n">
         <v>40</v>
       </c>
-      <c r="K3" s="19" t="n">
+      <c r="K3" s="20" t="n">
         <v>10</v>
       </c>
       <c r="L3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="I4" s="19" t="n">
+      <c r="I4" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="J4" s="19" t="n">
+      <c r="J4" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="K4" s="19" t="n">
+      <c r="K4" s="20" t="n">
         <v>3</v>
       </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="I5" s="19" t="n">
+      <c r="I5" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="J5" s="19" t="n">
+      <c r="J5" s="20" t="n">
         <v>40</v>
       </c>
-      <c r="K5" s="19" t="n">
+      <c r="K5" s="20" t="n">
         <v>10</v>
       </c>
       <c r="L5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="I6" s="19" t="n">
+      <c r="I6" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="J6" s="19" t="n">
+      <c r="J6" s="20" t="n">
         <v>40</v>
       </c>
-      <c r="K6" s="19" t="n">
+      <c r="K6" s="20" t="n">
         <v>10</v>
       </c>
       <c r="L6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="I7" s="19" t="n">
+      <c r="I7" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="J7" s="19" t="n">
+      <c r="J7" s="20" t="n">
         <v>40</v>
       </c>
-      <c r="K7" s="19" t="n">
+      <c r="K7" s="20" t="n">
         <v>10</v>
       </c>
       <c r="L7" s="2"/>
     </row>
     <row r="8" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="I8" s="19" t="n">
+      <c r="I8" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="J8" s="19" t="n">
+      <c r="J8" s="20" t="n">
         <v>40</v>
       </c>
-      <c r="K8" s="19" t="n">
+      <c r="K8" s="20" t="n">
         <v>10</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="12"/>
     </row>
     <row r="9" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="I9" s="19" t="n">
+      <c r="I9" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="J9" s="19" t="n">
+      <c r="J9" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="K9" s="19" t="n">
+      <c r="K9" s="20" t="n">
         <v>3</v>
       </c>
       <c r="L9" s="2"/>
@@ -3051,7 +3062,7 @@
   </sheetPr>
   <dimension ref="A1:XFD21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -3068,40 +3079,40 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>129</v>
       </c>
       <c r="XEW2" s="3"/>
@@ -3114,132 +3125,132 @@
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="F3" s="19" t="n">
+      <c r="F3" s="20" t="n">
         <v>0.167</v>
       </c>
-      <c r="G3" s="19" t="n">
+      <c r="G3" s="20" t="n">
         <v>0.167</v>
       </c>
-      <c r="H3" s="19" t="n">
+      <c r="H3" s="20" t="n">
         <v>0.167</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F4" s="19" t="n">
+      <c r="F4" s="20" t="n">
         <v>0.167</v>
       </c>
-      <c r="G4" s="19" t="n">
+      <c r="G4" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="H4" s="19" t="n">
+      <c r="H4" s="20" t="n">
         <v>0.583</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="19" t="n">
+      <c r="F5" s="20" t="n">
         <v>0.167</v>
       </c>
-      <c r="G5" s="19" t="n">
+      <c r="G5" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="H5" s="19" t="n">
+      <c r="H5" s="20" t="n">
         <v>0.583</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F6" s="19" t="n">
+      <c r="F6" s="20" t="n">
         <v>0.167</v>
       </c>
-      <c r="G6" s="19" t="n">
+      <c r="G6" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="H6" s="19" t="n">
+      <c r="H6" s="20" t="n">
         <v>0.583</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F7" s="19" t="n">
+      <c r="F7" s="20" t="n">
         <v>0.167</v>
       </c>
-      <c r="G7" s="19" t="n">
+      <c r="G7" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="19" t="n">
+      <c r="H7" s="20" t="n">
         <v>0.583</v>
       </c>
     </row>
@@ -3281,7 +3292,7 @@
   </sheetPr>
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -3303,200 +3314,200 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="P2" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="Q2" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="R2" s="21" t="s">
+      <c r="R2" s="22" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="D3" s="22" t="n">
+      <c r="D3" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="22" t="n">
+      <c r="E3" s="23" t="n">
         <v>15</v>
       </c>
-      <c r="F3" s="22" t="b">
+      <c r="F3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="H3" s="22" t="b">
+      <c r="H3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="J3" s="22" t="b">
+      <c r="J3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="L3" s="22" t="b">
+      <c r="L3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="N3" s="22" t="n">
+      <c r="N3" s="23" t="n">
         <v>4.5</v>
       </c>
-      <c r="O3" s="22" t="n">
+      <c r="O3" s="23" t="n">
         <v>1.5</v>
       </c>
-      <c r="P3" s="22" t="n">
+      <c r="P3" s="23" t="n">
         <v>250</v>
       </c>
-      <c r="Q3" s="22" t="n">
+      <c r="Q3" s="23" t="n">
         <v>200</v>
       </c>
-      <c r="R3" s="22" t="n">
+      <c r="R3" s="23" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="D4" s="22" t="n">
+      <c r="D4" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="E4" s="22" t="n">
+      <c r="E4" s="23" t="n">
         <v>12</v>
       </c>
-      <c r="F4" s="22" t="b">
+      <c r="F4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="H4" s="22" t="b">
+      <c r="H4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="J4" s="22" t="b">
+      <c r="J4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="L4" s="22" t="b">
+      <c r="L4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="N4" s="22" t="n">
+      <c r="N4" s="23" t="n">
         <v>6.5</v>
       </c>
-      <c r="O4" s="22" t="n">
+      <c r="O4" s="23" t="n">
         <v>2.5</v>
       </c>
-      <c r="P4" s="22" t="n">
+      <c r="P4" s="23" t="n">
         <v>400</v>
       </c>
-      <c r="Q4" s="22" t="n">
+      <c r="Q4" s="23" t="n">
         <v>350</v>
       </c>
-      <c r="R4" s="22" t="n">
+      <c r="R4" s="23" t="n">
         <v>25</v>
       </c>
     </row>
@@ -3558,92 +3569,92 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="22" t="s">
         <v>174</v>
       </c>
       <c r="L2" s="12"/>
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="22" t="b">
+      <c r="C3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="E3" s="22" t="b">
+      <c r="E3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="G3" s="22" t="b">
+      <c r="G3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="I3" s="22" t="n">
+      <c r="I3" s="23" t="n">
         <v>0.4</v>
       </c>
-      <c r="J3" s="22" t="n">
+      <c r="J3" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="K3" s="22" t="n">
+      <c r="K3" s="23" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change tracking setup. Modify central head/window use
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Mission" sheetId="1" state="visible" r:id="rId3"/>
@@ -94,28 +94,28 @@
     <t xml:space="preserve">(14:30:00)</t>
   </si>
   <si>
+    <t xml:space="preserve">MISSION01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coastal SAR Mission (Multi-Camera-Tracking)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENVIRONMENT01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUP02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PX4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(16:30:00)</t>
+  </si>
+  <si>
     <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MISSION01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coastal SAR Mission (Multi-Camera-Tracking)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENVIRONMENT01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GROUP02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEAM01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PX4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(16:30:00)</t>
   </si>
   <si>
     <t xml:space="preserve">MISSION02</t>
@@ -832,16 +832,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -905,7 +905,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
+          <fgColor rgb="FFDAE3F3"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -913,7 +913,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFDAE3F3"/>
+          <fgColor rgb="FF000000"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1375,8 +1375,8 @@
   </sheetPr>
   <dimension ref="A1:XFD19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1477,23 +1477,21 @@
       </c>
     </row>
     <row r="4" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="10" t="s">
         <v>25</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>16</v>
@@ -1502,73 +1500,75 @@
         <v>17</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12"/>
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="12"/>
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="12"/>
+      <c r="AM4" s="12"/>
+      <c r="AN4" s="12"/>
+      <c r="AO4" s="12"/>
+      <c r="AP4" s="12"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="12"/>
+      <c r="AS4" s="12"/>
+      <c r="AT4" s="12"/>
+      <c r="AU4" s="12"/>
+      <c r="AV4" s="12"/>
+      <c r="AW4" s="12"/>
+      <c r="AX4" s="12"/>
+      <c r="AY4" s="12"/>
+      <c r="AZ4" s="12"/>
+      <c r="BA4" s="12"/>
+      <c r="BB4" s="12"/>
+      <c r="BC4" s="12"/>
+      <c r="BD4" s="12"/>
+    </row>
+    <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="13"/>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="13"/>
-      <c r="AF4" s="13"/>
-      <c r="AG4" s="13"/>
-      <c r="AH4" s="13"/>
-      <c r="AI4" s="13"/>
-      <c r="AJ4" s="13"/>
-      <c r="AK4" s="13"/>
-      <c r="AL4" s="13"/>
-      <c r="AM4" s="13"/>
-      <c r="AN4" s="13"/>
-      <c r="AO4" s="13"/>
-      <c r="AP4" s="13"/>
-      <c r="AQ4" s="13"/>
-      <c r="AR4" s="13"/>
-      <c r="AS4" s="13"/>
-      <c r="AT4" s="13"/>
-      <c r="AU4" s="13"/>
-      <c r="AV4" s="13"/>
-      <c r="AW4" s="13"/>
-      <c r="AX4" s="13"/>
-      <c r="AY4" s="13"/>
-      <c r="AZ4" s="13"/>
-      <c r="BA4" s="13"/>
-      <c r="BB4" s="13"/>
-      <c r="BC4" s="13"/>
-      <c r="BD4" s="13"/>
-    </row>
-    <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11"/>
       <c r="B5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>31</v>
@@ -1580,59 +1580,59 @@
         <v>17</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13"/>
-      <c r="AH5" s="13"/>
-      <c r="AI5" s="13"/>
-      <c r="AJ5" s="13"/>
-      <c r="AK5" s="13"/>
-      <c r="AL5" s="13"/>
-      <c r="AM5" s="13"/>
-      <c r="AN5" s="13"/>
-      <c r="AO5" s="13"/>
-      <c r="AP5" s="13"/>
-      <c r="AQ5" s="13"/>
-      <c r="AR5" s="13"/>
-      <c r="AS5" s="13"/>
-      <c r="AT5" s="13"/>
-      <c r="AU5" s="13"/>
-      <c r="AV5" s="13"/>
-      <c r="AW5" s="13"/>
-      <c r="AX5" s="13"/>
-      <c r="AY5" s="13"/>
-      <c r="AZ5" s="13"/>
-      <c r="BA5" s="13"/>
-      <c r="BB5" s="13"/>
-      <c r="BC5" s="13"/>
-      <c r="BD5" s="13"/>
+        <v>27</v>
+      </c>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="12"/>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="12"/>
+      <c r="AH5" s="12"/>
+      <c r="AI5" s="12"/>
+      <c r="AJ5" s="12"/>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="12"/>
+      <c r="AM5" s="12"/>
+      <c r="AN5" s="12"/>
+      <c r="AO5" s="12"/>
+      <c r="AP5" s="12"/>
+      <c r="AQ5" s="12"/>
+      <c r="AR5" s="12"/>
+      <c r="AS5" s="12"/>
+      <c r="AT5" s="12"/>
+      <c r="AU5" s="12"/>
+      <c r="AV5" s="12"/>
+      <c r="AW5" s="12"/>
+      <c r="AX5" s="12"/>
+      <c r="AY5" s="12"/>
+      <c r="AZ5" s="12"/>
+      <c r="BA5" s="12"/>
+      <c r="BB5" s="12"/>
+      <c r="BC5" s="12"/>
+      <c r="BD5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G6" s="14"/>
@@ -1942,7 +1942,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="33.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="49.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="26.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="13" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="12" width="11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="6" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16382" style="3" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="2" width="10.49"/>
@@ -1955,7 +1955,7 @@
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
-      <c r="E1" s="13"/>
+      <c r="E1" s="12"/>
       <c r="XFB1" s="3"/>
       <c r="XFC1" s="3"/>
     </row>
@@ -1989,7 +1989,7 @@
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>37</v>
@@ -2119,63 +2119,63 @@
       <c r="G4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="13"/>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="13"/>
-      <c r="AF4" s="13"/>
-      <c r="AG4" s="13"/>
-      <c r="AH4" s="13"/>
-      <c r="AI4" s="13"/>
-      <c r="AJ4" s="13"/>
-      <c r="AK4" s="13"/>
-      <c r="AL4" s="13"/>
-      <c r="AM4" s="13"/>
-      <c r="AN4" s="13"/>
-      <c r="AO4" s="13"/>
-      <c r="AP4" s="13"/>
-      <c r="AQ4" s="13"/>
-      <c r="AR4" s="13"/>
-      <c r="AS4" s="13"/>
-      <c r="AT4" s="13"/>
-      <c r="AU4" s="13"/>
-      <c r="AV4" s="13"/>
-      <c r="AW4" s="13"/>
-      <c r="AX4" s="13"/>
-      <c r="AY4" s="13"/>
-      <c r="AZ4" s="13"/>
-      <c r="BA4" s="13"/>
-      <c r="BB4" s="13"/>
-      <c r="BC4" s="13"/>
-      <c r="BD4" s="13"/>
-      <c r="BE4" s="13"/>
-      <c r="BF4" s="13"/>
-      <c r="BG4" s="13"/>
-      <c r="BH4" s="13"/>
-      <c r="BI4" s="13"/>
-      <c r="BJ4" s="13"/>
-      <c r="BK4" s="13"/>
-      <c r="BL4" s="13"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12"/>
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="12"/>
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="12"/>
+      <c r="AM4" s="12"/>
+      <c r="AN4" s="12"/>
+      <c r="AO4" s="12"/>
+      <c r="AP4" s="12"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="12"/>
+      <c r="AS4" s="12"/>
+      <c r="AT4" s="12"/>
+      <c r="AU4" s="12"/>
+      <c r="AV4" s="12"/>
+      <c r="AW4" s="12"/>
+      <c r="AX4" s="12"/>
+      <c r="AY4" s="12"/>
+      <c r="AZ4" s="12"/>
+      <c r="BA4" s="12"/>
+      <c r="BB4" s="12"/>
+      <c r="BC4" s="12"/>
+      <c r="BD4" s="12"/>
+      <c r="BE4" s="12"/>
+      <c r="BF4" s="12"/>
+      <c r="BG4" s="12"/>
+      <c r="BH4" s="12"/>
+      <c r="BI4" s="12"/>
+      <c r="BJ4" s="12"/>
+      <c r="BK4" s="12"/>
+      <c r="BL4" s="12"/>
       <c r="BM4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2186,7 +2186,7 @@
         <v>53</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>51</v>
@@ -2200,63 +2200,63 @@
       <c r="G5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13"/>
-      <c r="AH5" s="13"/>
-      <c r="AI5" s="13"/>
-      <c r="AJ5" s="13"/>
-      <c r="AK5" s="13"/>
-      <c r="AL5" s="13"/>
-      <c r="AM5" s="13"/>
-      <c r="AN5" s="13"/>
-      <c r="AO5" s="13"/>
-      <c r="AP5" s="13"/>
-      <c r="AQ5" s="13"/>
-      <c r="AR5" s="13"/>
-      <c r="AS5" s="13"/>
-      <c r="AT5" s="13"/>
-      <c r="AU5" s="13"/>
-      <c r="AV5" s="13"/>
-      <c r="AW5" s="13"/>
-      <c r="AX5" s="13"/>
-      <c r="AY5" s="13"/>
-      <c r="AZ5" s="13"/>
-      <c r="BA5" s="13"/>
-      <c r="BB5" s="13"/>
-      <c r="BC5" s="13"/>
-      <c r="BD5" s="13"/>
-      <c r="BE5" s="13"/>
-      <c r="BF5" s="13"/>
-      <c r="BG5" s="13"/>
-      <c r="BH5" s="13"/>
-      <c r="BI5" s="13"/>
-      <c r="BJ5" s="13"/>
-      <c r="BK5" s="13"/>
-      <c r="BL5" s="13"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="12"/>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="12"/>
+      <c r="AH5" s="12"/>
+      <c r="AI5" s="12"/>
+      <c r="AJ5" s="12"/>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="12"/>
+      <c r="AM5" s="12"/>
+      <c r="AN5" s="12"/>
+      <c r="AO5" s="12"/>
+      <c r="AP5" s="12"/>
+      <c r="AQ5" s="12"/>
+      <c r="AR5" s="12"/>
+      <c r="AS5" s="12"/>
+      <c r="AT5" s="12"/>
+      <c r="AU5" s="12"/>
+      <c r="AV5" s="12"/>
+      <c r="AW5" s="12"/>
+      <c r="AX5" s="12"/>
+      <c r="AY5" s="12"/>
+      <c r="AZ5" s="12"/>
+      <c r="BA5" s="12"/>
+      <c r="BB5" s="12"/>
+      <c r="BC5" s="12"/>
+      <c r="BD5" s="12"/>
+      <c r="BE5" s="12"/>
+      <c r="BF5" s="12"/>
+      <c r="BG5" s="12"/>
+      <c r="BH5" s="12"/>
+      <c r="BI5" s="12"/>
+      <c r="BJ5" s="12"/>
+      <c r="BK5" s="12"/>
+      <c r="BL5" s="12"/>
       <c r="BM5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2294,16 +2294,16 @@
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="38.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="38.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="13" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="12" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="29.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="36.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="29.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="14" style="13" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="14" style="12" width="11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="19" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="2" width="10.49"/>
   </cols>
@@ -2361,11 +2361,11 @@
       <c r="L2" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
     </row>
     <row r="3" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
@@ -2405,13 +2405,13 @@
         <v>12000</v>
       </c>
       <c r="M3" s="2"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
       <c r="XFB3" s="2"/>
       <c r="XFC3" s="2"/>
       <c r="XFD3" s="2"/>
@@ -2424,7 +2424,7 @@
         <v>74</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>67</v>
@@ -2540,12 +2540,12 @@
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="38.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="13" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="38.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="12" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="29.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="8" style="13" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="8" style="12" width="11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16375" min="13" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16378" min="16376" style="2" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16379" style="3" width="10.49"/>
@@ -2580,11 +2580,11 @@
       <c r="F2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
       <c r="XEY2" s="3"/>
       <c r="XEZ2" s="3"/>
       <c r="XFA2" s="3"/>
@@ -2612,13 +2612,13 @@
         <v>0.6</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
       <c r="XEV3" s="2"/>
       <c r="XEW3" s="2"/>
       <c r="XEX3" s="2"/>
@@ -2643,13 +2643,13 @@
         <v>0.6</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
       <c r="XEV4" s="2"/>
       <c r="XEW4" s="2"/>
       <c r="XEX4" s="2"/>
@@ -2696,7 +2696,7 @@
   </sheetPr>
   <dimension ref="A1:XFD26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -2705,10 +2705,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="38.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="13" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="12" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="36.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="13" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="12" width="11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="15" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="3" width="10.49"/>
   </cols>
@@ -2763,7 +2763,7 @@
       <c r="K2" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="M2" s="13"/>
+      <c r="M2" s="12"/>
       <c r="N2" s="3"/>
       <c r="XFD2" s="3"/>
     </row>
@@ -2982,7 +2982,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="M8" s="13"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
@@ -3019,7 +3019,7 @@
         <v>3</v>
       </c>
       <c r="L9" s="2"/>
-      <c r="M9" s="13"/>
+      <c r="M9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3071,9 +3071,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="38.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="12" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="13" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="12" width="27.34"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16376" min="9" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16377" style="3" width="10.49"/>
   </cols>
@@ -3304,11 +3304,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="28.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="64.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="29.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="13" width="51.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="13" width="37.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="12" width="51.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="12" width="37.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="54.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="13" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="12" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="2" width="26.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="19" style="2" width="11"/>
   </cols>
@@ -3564,7 +3564,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="29.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="40.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="2" width="29.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="13" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="12" width="11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="13" style="2" width="11"/>
   </cols>
   <sheetData>
@@ -3617,7 +3617,7 @@
       <c r="K2" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="L2" s="13"/>
+      <c r="L2" s="12"/>
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Create auxiliary frame to compute tracking orientation
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -832,16 +832,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1376,7 +1376,7 @@
   <dimension ref="A1:XFD19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1477,11 +1477,11 @@
       </c>
     </row>
     <row r="4" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -1508,60 +1508,60 @@
       <c r="K4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="12"/>
-      <c r="AC4" s="12"/>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="12"/>
-      <c r="AF4" s="12"/>
-      <c r="AG4" s="12"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="12"/>
-      <c r="AJ4" s="12"/>
-      <c r="AK4" s="12"/>
-      <c r="AL4" s="12"/>
-      <c r="AM4" s="12"/>
-      <c r="AN4" s="12"/>
-      <c r="AO4" s="12"/>
-      <c r="AP4" s="12"/>
-      <c r="AQ4" s="12"/>
-      <c r="AR4" s="12"/>
-      <c r="AS4" s="12"/>
-      <c r="AT4" s="12"/>
-      <c r="AU4" s="12"/>
-      <c r="AV4" s="12"/>
-      <c r="AW4" s="12"/>
-      <c r="AX4" s="12"/>
-      <c r="AY4" s="12"/>
-      <c r="AZ4" s="12"/>
-      <c r="BA4" s="12"/>
-      <c r="BB4" s="12"/>
-      <c r="BC4" s="12"/>
-      <c r="BD4" s="12"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="13"/>
+      <c r="AC4" s="13"/>
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="13"/>
+      <c r="AF4" s="13"/>
+      <c r="AG4" s="13"/>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="13"/>
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="13"/>
+      <c r="AL4" s="13"/>
+      <c r="AM4" s="13"/>
+      <c r="AN4" s="13"/>
+      <c r="AO4" s="13"/>
+      <c r="AP4" s="13"/>
+      <c r="AQ4" s="13"/>
+      <c r="AR4" s="13"/>
+      <c r="AS4" s="13"/>
+      <c r="AT4" s="13"/>
+      <c r="AU4" s="13"/>
+      <c r="AV4" s="13"/>
+      <c r="AW4" s="13"/>
+      <c r="AX4" s="13"/>
+      <c r="AY4" s="13"/>
+      <c r="AZ4" s="13"/>
+      <c r="BA4" s="13"/>
+      <c r="BB4" s="13"/>
+      <c r="BC4" s="13"/>
+      <c r="BD4" s="13"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1588,51 +1588,51 @@
       <c r="K5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="12"/>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="12"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="12"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="12"/>
-      <c r="AJ5" s="12"/>
-      <c r="AK5" s="12"/>
-      <c r="AL5" s="12"/>
-      <c r="AM5" s="12"/>
-      <c r="AN5" s="12"/>
-      <c r="AO5" s="12"/>
-      <c r="AP5" s="12"/>
-      <c r="AQ5" s="12"/>
-      <c r="AR5" s="12"/>
-      <c r="AS5" s="12"/>
-      <c r="AT5" s="12"/>
-      <c r="AU5" s="12"/>
-      <c r="AV5" s="12"/>
-      <c r="AW5" s="12"/>
-      <c r="AX5" s="12"/>
-      <c r="AY5" s="12"/>
-      <c r="AZ5" s="12"/>
-      <c r="BA5" s="12"/>
-      <c r="BB5" s="12"/>
-      <c r="BC5" s="12"/>
-      <c r="BD5" s="12"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="13"/>
+      <c r="AN5" s="13"/>
+      <c r="AO5" s="13"/>
+      <c r="AP5" s="13"/>
+      <c r="AQ5" s="13"/>
+      <c r="AR5" s="13"/>
+      <c r="AS5" s="13"/>
+      <c r="AT5" s="13"/>
+      <c r="AU5" s="13"/>
+      <c r="AV5" s="13"/>
+      <c r="AW5" s="13"/>
+      <c r="AX5" s="13"/>
+      <c r="AY5" s="13"/>
+      <c r="AZ5" s="13"/>
+      <c r="BA5" s="13"/>
+      <c r="BB5" s="13"/>
+      <c r="BC5" s="13"/>
+      <c r="BD5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G6" s="14"/>
@@ -1942,7 +1942,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="33.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="49.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="26.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="12" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="13" width="11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="6" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16382" style="3" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="2" width="10.49"/>
@@ -1955,7 +1955,7 @@
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
-      <c r="E1" s="12"/>
+      <c r="E1" s="13"/>
       <c r="XFB1" s="3"/>
       <c r="XFC1" s="3"/>
     </row>
@@ -2119,63 +2119,63 @@
       <c r="G4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="12"/>
-      <c r="AC4" s="12"/>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="12"/>
-      <c r="AF4" s="12"/>
-      <c r="AG4" s="12"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="12"/>
-      <c r="AJ4" s="12"/>
-      <c r="AK4" s="12"/>
-      <c r="AL4" s="12"/>
-      <c r="AM4" s="12"/>
-      <c r="AN4" s="12"/>
-      <c r="AO4" s="12"/>
-      <c r="AP4" s="12"/>
-      <c r="AQ4" s="12"/>
-      <c r="AR4" s="12"/>
-      <c r="AS4" s="12"/>
-      <c r="AT4" s="12"/>
-      <c r="AU4" s="12"/>
-      <c r="AV4" s="12"/>
-      <c r="AW4" s="12"/>
-      <c r="AX4" s="12"/>
-      <c r="AY4" s="12"/>
-      <c r="AZ4" s="12"/>
-      <c r="BA4" s="12"/>
-      <c r="BB4" s="12"/>
-      <c r="BC4" s="12"/>
-      <c r="BD4" s="12"/>
-      <c r="BE4" s="12"/>
-      <c r="BF4" s="12"/>
-      <c r="BG4" s="12"/>
-      <c r="BH4" s="12"/>
-      <c r="BI4" s="12"/>
-      <c r="BJ4" s="12"/>
-      <c r="BK4" s="12"/>
-      <c r="BL4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="13"/>
+      <c r="AC4" s="13"/>
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="13"/>
+      <c r="AF4" s="13"/>
+      <c r="AG4" s="13"/>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="13"/>
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="13"/>
+      <c r="AL4" s="13"/>
+      <c r="AM4" s="13"/>
+      <c r="AN4" s="13"/>
+      <c r="AO4" s="13"/>
+      <c r="AP4" s="13"/>
+      <c r="AQ4" s="13"/>
+      <c r="AR4" s="13"/>
+      <c r="AS4" s="13"/>
+      <c r="AT4" s="13"/>
+      <c r="AU4" s="13"/>
+      <c r="AV4" s="13"/>
+      <c r="AW4" s="13"/>
+      <c r="AX4" s="13"/>
+      <c r="AY4" s="13"/>
+      <c r="AZ4" s="13"/>
+      <c r="BA4" s="13"/>
+      <c r="BB4" s="13"/>
+      <c r="BC4" s="13"/>
+      <c r="BD4" s="13"/>
+      <c r="BE4" s="13"/>
+      <c r="BF4" s="13"/>
+      <c r="BG4" s="13"/>
+      <c r="BH4" s="13"/>
+      <c r="BI4" s="13"/>
+      <c r="BJ4" s="13"/>
+      <c r="BK4" s="13"/>
+      <c r="BL4" s="13"/>
       <c r="BM4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2200,63 +2200,63 @@
       <c r="G5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="12"/>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="12"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="12"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="12"/>
-      <c r="AJ5" s="12"/>
-      <c r="AK5" s="12"/>
-      <c r="AL5" s="12"/>
-      <c r="AM5" s="12"/>
-      <c r="AN5" s="12"/>
-      <c r="AO5" s="12"/>
-      <c r="AP5" s="12"/>
-      <c r="AQ5" s="12"/>
-      <c r="AR5" s="12"/>
-      <c r="AS5" s="12"/>
-      <c r="AT5" s="12"/>
-      <c r="AU5" s="12"/>
-      <c r="AV5" s="12"/>
-      <c r="AW5" s="12"/>
-      <c r="AX5" s="12"/>
-      <c r="AY5" s="12"/>
-      <c r="AZ5" s="12"/>
-      <c r="BA5" s="12"/>
-      <c r="BB5" s="12"/>
-      <c r="BC5" s="12"/>
-      <c r="BD5" s="12"/>
-      <c r="BE5" s="12"/>
-      <c r="BF5" s="12"/>
-      <c r="BG5" s="12"/>
-      <c r="BH5" s="12"/>
-      <c r="BI5" s="12"/>
-      <c r="BJ5" s="12"/>
-      <c r="BK5" s="12"/>
-      <c r="BL5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="13"/>
+      <c r="AN5" s="13"/>
+      <c r="AO5" s="13"/>
+      <c r="AP5" s="13"/>
+      <c r="AQ5" s="13"/>
+      <c r="AR5" s="13"/>
+      <c r="AS5" s="13"/>
+      <c r="AT5" s="13"/>
+      <c r="AU5" s="13"/>
+      <c r="AV5" s="13"/>
+      <c r="AW5" s="13"/>
+      <c r="AX5" s="13"/>
+      <c r="AY5" s="13"/>
+      <c r="AZ5" s="13"/>
+      <c r="BA5" s="13"/>
+      <c r="BB5" s="13"/>
+      <c r="BC5" s="13"/>
+      <c r="BD5" s="13"/>
+      <c r="BE5" s="13"/>
+      <c r="BF5" s="13"/>
+      <c r="BG5" s="13"/>
+      <c r="BH5" s="13"/>
+      <c r="BI5" s="13"/>
+      <c r="BJ5" s="13"/>
+      <c r="BK5" s="13"/>
+      <c r="BL5" s="13"/>
       <c r="BM5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2294,16 +2294,16 @@
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="38.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="38.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="12" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="13" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="29.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="36.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="29.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="14" style="12" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="14" style="13" width="11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="19" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="2" width="10.49"/>
   </cols>
@@ -2361,11 +2361,11 @@
       <c r="L2" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
     </row>
     <row r="3" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
@@ -2405,13 +2405,13 @@
         <v>12000</v>
       </c>
       <c r="M3" s="2"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
       <c r="XFB3" s="2"/>
       <c r="XFC3" s="2"/>
       <c r="XFD3" s="2"/>
@@ -2540,12 +2540,12 @@
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="38.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="12" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="38.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="13" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="29.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="8" style="12" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="8" style="13" width="11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16375" min="13" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16378" min="16376" style="2" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16379" style="3" width="10.49"/>
@@ -2580,11 +2580,11 @@
       <c r="F2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
       <c r="XEY2" s="3"/>
       <c r="XEZ2" s="3"/>
       <c r="XFA2" s="3"/>
@@ -2612,13 +2612,13 @@
         <v>0.6</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
       <c r="XEV3" s="2"/>
       <c r="XEW3" s="2"/>
       <c r="XEX3" s="2"/>
@@ -2643,13 +2643,13 @@
         <v>0.6</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
       <c r="XEV4" s="2"/>
       <c r="XEW4" s="2"/>
       <c r="XEX4" s="2"/>
@@ -2705,10 +2705,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="38.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="12" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="13" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="36.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="12" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="13" width="11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="15" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="3" width="10.49"/>
   </cols>
@@ -2763,7 +2763,7 @@
       <c r="K2" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="M2" s="12"/>
+      <c r="M2" s="13"/>
       <c r="N2" s="3"/>
       <c r="XFD2" s="3"/>
     </row>
@@ -2982,7 +2982,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="M8" s="12"/>
+      <c r="M8" s="13"/>
     </row>
     <row r="9" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
@@ -3019,7 +3019,7 @@
         <v>3</v>
       </c>
       <c r="L9" s="2"/>
-      <c r="M9" s="12"/>
+      <c r="M9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3071,9 +3071,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="38.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="12" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="12" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="13" width="27.34"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16376" min="9" style="2" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16377" style="3" width="10.49"/>
   </cols>
@@ -3304,11 +3304,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="28.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="64.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="29.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="12" width="51.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="12" width="37.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="13" width="51.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="13" width="37.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="54.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="12" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="13" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="2" width="26.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="19" style="2" width="11"/>
   </cols>
@@ -3564,7 +3564,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="29.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="40.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="2" width="29.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="12" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="13" width="11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="13" style="2" width="11"/>
   </cols>
   <sheetData>
@@ -3617,7 +3617,7 @@
       <c r="K2" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="L2" s="12"/>
+      <c r="L2" s="13"/>
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add camera scale setting
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="197">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">(-150.0, 150.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">(30.0, 150.0)</t>
+    <t xml:space="preserve">(50.0, 150.0)</t>
   </si>
   <si>
     <t xml:space="preserve">SimpleFlight</t>
@@ -94,6 +94,9 @@
     <t xml:space="preserve">(14:30:00)</t>
   </si>
   <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
     <t xml:space="preserve">MISSION01</t>
   </si>
   <si>
@@ -115,9 +118,6 @@
     <t xml:space="preserve">(16:30:00)</t>
   </si>
   <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
     <t xml:space="preserve">MISSION02</t>
   </si>
   <si>
@@ -352,6 +352,9 @@
     <t xml:space="preserve">Central</t>
   </si>
   <si>
+    <t xml:space="preserve">(X=0.0, Y=0.0, Z=-0.09)</t>
+  </si>
+  <si>
     <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=90.0)</t>
   </si>
   <si>
@@ -364,7 +367,35 @@
     <t xml:space="preserve">CAM01</t>
   </si>
   <si>
-    <t xml:space="preserve">(X=0.3, Y=0.0, Z=-0.15)</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(X=0.2, Y=-0.18, Z=-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">0.09</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">HEAD03</t>
@@ -373,7 +404,35 @@
     <t xml:space="preserve">Multi-Camera Tracking Head 2</t>
   </si>
   <si>
-    <t xml:space="preserve">(X=0.0, Y=0.3, Z=-0.15)</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(X=0.2, Y=0.18, Z=-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">0.09</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">HEAD04</t>
@@ -382,7 +441,35 @@
     <t xml:space="preserve">Multi-Camera Tracking Head 3</t>
   </si>
   <si>
-    <t xml:space="preserve">(X=-0.3, Y=0.0, Z=-0.15)</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(X=-0.2, Y=0.18, Z=-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">0.09</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=180.0)</t>
@@ -394,7 +481,35 @@
     <t xml:space="preserve">Multi-Camera Tracking Head 4</t>
   </si>
   <si>
-    <t xml:space="preserve">(X=0.0, Y=-0.3, Z=-0.15)</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(X=-0.2, Y=-0.18, Z=-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">0.09</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=270.0)</t>
@@ -407,6 +522,37 @@
   </si>
   <si>
     <t xml:space="preserve">CAM03</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(X=0.0, Y=0.0, Z=-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">0.09</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Resolution [pix]</t>
@@ -625,7 +771,7 @@
     <numFmt numFmtId="165" formatCode="h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -698,6 +844,12 @@
       <b val="true"/>
       <sz val="16"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -905,7 +1057,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFDAE3F3"/>
+          <fgColor rgb="FF000000"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -913,7 +1065,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
+          <fgColor rgb="FFDAE3F3"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1376,7 +1528,7 @@
   <dimension ref="A1:XFD19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1477,21 +1629,23 @@
       </c>
     </row>
     <row r="4" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11"/>
+      <c r="A4" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="B4" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>16</v>
@@ -1500,13 +1654,13 @@
         <v>17</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
@@ -1555,9 +1709,7 @@
       <c r="BD4" s="13"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>28</v>
-      </c>
+      <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
         <v>29</v>
       </c>
@@ -1565,10 +1717,10 @@
         <v>30</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>31</v>
@@ -1580,13 +1732,13 @@
         <v>17</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
@@ -1679,7 +1831,7 @@
   <dimension ref="A1:XFD20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1699,7 +1851,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -1723,28 +1875,28 @@
         <v>39</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="XFB2" s="3"/>
       <c r="XFC2" s="3"/>
@@ -1755,26 +1907,26 @@
         <v>99</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I3" s="23" t="n">
         <v>0.5</v>
@@ -1788,29 +1940,29 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>188</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>186</v>
       </c>
       <c r="G4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I4" s="23" t="n">
         <v>0.5</v>
@@ -1827,26 +1979,26 @@
         <v>105</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G5" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I5" s="23" t="n">
         <v>0.2</v>
@@ -1860,29 +2012,29 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G6" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I6" s="23" t="n">
         <v>0.8</v>
@@ -1933,7 +2085,7 @@
   <dimension ref="A1:XFC4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1989,7 +2141,7 @@
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>37</v>
@@ -2186,7 +2338,7 @@
         <v>53</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>51</v>
@@ -2287,8 +2439,8 @@
   </sheetPr>
   <dimension ref="A1:XFD22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2424,7 +2576,7 @@
         <v>74</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>67</v>
@@ -2534,7 +2686,7 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2609,7 +2761,7 @@
         <v>0.9</v>
       </c>
       <c r="F3" s="20" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="13"/>
@@ -2640,7 +2792,7 @@
         <v>0.9</v>
       </c>
       <c r="F4" s="20" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="13"/>
@@ -2697,7 +2849,7 @@
   <dimension ref="A1:XFD26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2823,28 +2975,28 @@
         <v>106</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I4" s="20" t="n">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="J4" s="20" t="n">
         <v>3</v>
       </c>
       <c r="K4" s="20" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>75</v>
@@ -2853,13 +3005,13 @@
         <v>98</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>100</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>102</v>
@@ -2877,10 +3029,10 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>75</v>
@@ -2889,16 +3041,16 @@
         <v>98</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>100</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I6" s="20" t="n">
         <v>8</v>
@@ -2913,10 +3065,10 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>75</v>
@@ -2925,16 +3077,16 @@
         <v>98</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F7" s="20" t="s">
         <v>100</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I7" s="20" t="n">
         <v>8</v>
@@ -2949,10 +3101,10 @@
     </row>
     <row r="8" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>75</v>
@@ -2961,16 +3113,16 @@
         <v>98</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>100</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I8" s="20" t="n">
         <v>8</v>
@@ -2986,10 +3138,10 @@
     </row>
     <row r="9" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>80</v>
@@ -2998,25 +3150,25 @@
         <v>98</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F9" s="20" t="s">
         <v>106</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I9" s="20" t="n">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="J9" s="20" t="n">
         <v>3</v>
       </c>
       <c r="K9" s="20" t="n">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="13"/>
@@ -3063,7 +3215,7 @@
   <dimension ref="A1:XFD21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3104,16 +3256,16 @@
         <v>92</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="XEW2" s="3"/>
       <c r="XEX2" s="3"/>
@@ -3126,10 +3278,10 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>81</v>
@@ -3138,7 +3290,7 @@
         <v>106</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F3" s="20" t="n">
         <v>0.167</v>
@@ -3152,10 +3304,10 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>81</v>
@@ -3164,7 +3316,7 @@
         <v>100</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F4" s="20" t="n">
         <v>0.167</v>
@@ -3178,10 +3330,10 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>81</v>
@@ -3190,7 +3342,7 @@
         <v>100</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F5" s="20" t="n">
         <v>0.167</v>
@@ -3204,10 +3356,10 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>81</v>
@@ -3216,7 +3368,7 @@
         <v>100</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F6" s="20" t="n">
         <v>0.167</v>
@@ -3230,10 +3382,10 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>81</v>
@@ -3242,7 +3394,7 @@
         <v>100</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F7" s="20" t="n">
         <v>0.167</v>
@@ -3315,7 +3467,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -3346,49 +3498,49 @@
         <v>39</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="N2" s="22" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="O2" s="22" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="P2" s="22" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="Q2" s="22" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="R2" s="22" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3396,10 +3548,10 @@
         <v>70</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D3" s="23" t="n">
         <v>10</v>
@@ -3412,28 +3564,28 @@
         <v>1</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="L3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M3" s="23" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="N3" s="23" t="n">
         <v>4.5</v>
@@ -3456,10 +3608,10 @@
         <v>76</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D4" s="23" t="n">
         <v>8</v>
@@ -3472,28 +3624,28 @@
         <v>1</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="L4" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M4" s="23" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="N4" s="23" t="n">
         <v>6.5</v>
@@ -3570,7 +3722,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -3591,31 +3743,31 @@
         <v>2</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="L2" s="13"/>
       <c r="XFD2" s="3"/>
@@ -3625,28 +3777,28 @@
         <v>98</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G3" s="23" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="I3" s="23" t="n">
         <v>0.4</v>

</xml_diff>